<commit_message>
Actualización escaletas 11_02 y 11_03
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion01/Escaleta_CN_11_01_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion01/Escaleta_CN_11_01_CO.xlsx
@@ -18,8 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$2</definedName>
   </definedNames>
-  <calcPr calcId="140001"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -643,7 +642,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -673,12 +672,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -856,7 +849,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -878,233 +871,230 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1412,168 +1402,180 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
+      <selection pane="bottomLeft" activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="8.85546875" style="45"/>
-    <col min="4" max="4" width="33" style="45" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.5703125" style="45" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="84"/>
-    <col min="7" max="7" width="75.28515625" style="45" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.85546875" style="84"/>
-    <col min="10" max="10" width="10.85546875" style="45" customWidth="1"/>
-    <col min="11" max="14" width="8.85546875" style="45"/>
-    <col min="15" max="17" width="8.85546875" style="84"/>
-    <col min="18" max="16384" width="8.85546875" style="45"/>
+    <col min="1" max="1" width="13" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" style="60" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="75.28515625" style="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" style="60" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" style="60" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="112.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.28515625" style="22" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" style="22" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="153.7109375" style="60" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.42578125" style="60" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.140625" style="60" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="44.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.85546875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="21" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:21" s="9" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="67" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="65" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="61" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="61" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="61" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="71" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="16"/>
-      <c r="O1" s="17" t="s">
+      <c r="N1" s="75"/>
+      <c r="O1" s="63" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="17" t="s">
+      <c r="P1" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="18" t="s">
+      <c r="Q1" s="78" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="19" t="s">
+      <c r="R1" s="82" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="18" t="s">
+      <c r="S1" s="78" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="20" t="s">
+      <c r="T1" s="80" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="18" t="s">
+      <c r="U1" s="78" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="21" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="29" t="s">
+    <row r="2" spans="1:21" s="9" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="68"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="N2" s="29" t="s">
+      <c r="N2" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="31"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="64"/>
+      <c r="Q2" s="79"/>
+      <c r="R2" s="83"/>
+      <c r="S2" s="79"/>
+      <c r="T2" s="81"/>
+      <c r="U2" s="79"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="E3" s="35"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="39" t="s">
+      <c r="E3" s="12"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="H3" s="38">
+      <c r="H3" s="15">
         <v>1</v>
       </c>
-      <c r="I3" s="38" t="s">
+      <c r="I3" s="15" t="s">
         <v>19</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="K3" s="40" t="s">
+      <c r="K3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="39" t="s">
+      <c r="L3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="41" t="s">
+      <c r="M3" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="N3" s="41"/>
-      <c r="O3" s="42" t="s">
+      <c r="N3" s="18"/>
+      <c r="O3" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="P3" s="42" t="s">
+      <c r="P3" s="19" t="s">
         <v>19</v>
       </c>
       <c r="Q3" s="3">
         <v>6</v>
       </c>
-      <c r="R3" s="43" t="s">
+      <c r="R3" s="20" t="s">
         <v>167</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="T3" s="44" t="s">
+      <c r="T3" s="21" t="s">
         <v>169</v>
       </c>
       <c r="U3" s="3" t="s">
@@ -1581,56 +1583,56 @@
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="E4" s="46" t="s">
+      <c r="E4" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="F4" s="47"/>
-      <c r="G4" s="39" t="s">
+      <c r="F4" s="24"/>
+      <c r="G4" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="H4" s="38">
+      <c r="H4" s="15">
         <v>2</v>
       </c>
-      <c r="I4" s="48" t="s">
+      <c r="I4" s="25" t="s">
         <v>20</v>
       </c>
       <c r="J4" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="K4" s="49" t="s">
+      <c r="K4" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="50" t="s">
+      <c r="L4" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51" t="s">
+      <c r="M4" s="28"/>
+      <c r="N4" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="O4" s="47"/>
-      <c r="P4" s="47"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
       <c r="Q4" s="4">
         <v>6</v>
       </c>
-      <c r="R4" s="52" t="s">
+      <c r="R4" s="29" t="s">
         <v>171</v>
       </c>
       <c r="S4" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="T4" s="53" t="s">
+      <c r="T4" s="30" t="s">
         <v>173</v>
       </c>
       <c r="U4" s="4" t="s">
@@ -1638,227 +1640,227 @@
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="F5" s="47"/>
-      <c r="G5" s="39" t="s">
+      <c r="F5" s="24"/>
+      <c r="G5" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="H5" s="38">
+      <c r="H5" s="15">
         <v>3</v>
       </c>
-      <c r="I5" s="48" t="s">
+      <c r="I5" s="25" t="s">
         <v>20</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="K5" s="49" t="s">
+      <c r="K5" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="L5" s="50" t="s">
+      <c r="L5" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="M5" s="51"/>
-      <c r="N5" s="51"/>
-      <c r="O5" s="47" t="s">
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="P5" s="47"/>
-      <c r="Q5" s="4">
+      <c r="P5" s="24"/>
+      <c r="Q5" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="R5" s="20">
         <v>8</v>
       </c>
-      <c r="R5" s="52" t="s">
-        <v>134</v>
-      </c>
-      <c r="S5" s="4" t="s">
+      <c r="S5" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="T5" s="53" t="s">
+      <c r="T5" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="U5" s="54" t="s">
+      <c r="U5" s="3" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="E6" s="46" t="s">
+      <c r="E6" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="F6" s="47"/>
-      <c r="G6" s="39" t="s">
+      <c r="F6" s="24"/>
+      <c r="G6" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="H6" s="38">
+      <c r="H6" s="15">
         <v>4</v>
       </c>
-      <c r="I6" s="48" t="s">
+      <c r="I6" s="25" t="s">
         <v>20</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="K6" s="49" t="s">
+      <c r="K6" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="L6" s="50" t="s">
+      <c r="L6" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="51"/>
-      <c r="N6" s="51" t="s">
+      <c r="M6" s="28"/>
+      <c r="N6" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="O6" s="47"/>
-      <c r="P6" s="47"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
       <c r="Q6" s="3">
         <v>6</v>
       </c>
-      <c r="R6" s="43" t="s">
+      <c r="R6" s="20" t="s">
         <v>171</v>
       </c>
       <c r="S6" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="T6" s="44" t="s">
+      <c r="T6" s="21" t="s">
         <v>176</v>
       </c>
       <c r="U6" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="56" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+    <row r="7" spans="1:21" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="E7" s="55" t="s">
+      <c r="E7" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="F7" s="47"/>
-      <c r="G7" s="39" t="s">
+      <c r="F7" s="24"/>
+      <c r="G7" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="H7" s="38">
+      <c r="H7" s="15">
         <v>5</v>
       </c>
-      <c r="I7" s="48" t="s">
+      <c r="I7" s="25" t="s">
         <v>20</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="K7" s="49" t="s">
+      <c r="K7" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="L7" s="50" t="s">
+      <c r="L7" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="51"/>
-      <c r="N7" s="51" t="s">
+      <c r="M7" s="28"/>
+      <c r="N7" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="O7" s="47"/>
-      <c r="P7" s="47"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="24"/>
       <c r="Q7" s="3">
         <v>6</v>
       </c>
-      <c r="R7" s="43" t="s">
+      <c r="R7" s="20" t="s">
         <v>171</v>
       </c>
       <c r="S7" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="T7" s="44" t="s">
+      <c r="T7" s="21" t="s">
         <v>177</v>
       </c>
       <c r="U7" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="70" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="57" t="s">
+    <row r="8" spans="1:21" s="46" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="58" t="s">
+      <c r="B8" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="C8" s="59" t="s">
+      <c r="C8" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="D8" s="57" t="s">
+      <c r="D8" s="33" t="s">
         <v>158</v>
       </c>
-      <c r="E8" s="60" t="s">
+      <c r="E8" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="F8" s="61"/>
-      <c r="G8" s="62" t="s">
+      <c r="F8" s="37"/>
+      <c r="G8" s="38" t="s">
         <v>148</v>
       </c>
-      <c r="H8" s="63">
+      <c r="H8" s="39">
         <v>6</v>
       </c>
-      <c r="I8" s="64" t="s">
+      <c r="I8" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="65" t="s">
+      <c r="J8" s="41" t="s">
         <v>192</v>
       </c>
-      <c r="K8" s="66" t="s">
+      <c r="K8" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="62" t="s">
+      <c r="L8" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="M8" s="67"/>
-      <c r="N8" s="67" t="s">
+      <c r="M8" s="43"/>
+      <c r="N8" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="O8" s="61"/>
-      <c r="P8" s="61"/>
+      <c r="O8" s="37"/>
+      <c r="P8" s="37"/>
       <c r="Q8" s="6">
         <v>6</v>
       </c>
-      <c r="R8" s="68" t="s">
+      <c r="R8" s="44" t="s">
         <v>171</v>
       </c>
       <c r="S8" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="T8" s="69" t="s">
+      <c r="T8" s="45" t="s">
         <v>178</v>
       </c>
       <c r="U8" s="6" t="s">
@@ -1866,54 +1868,54 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="D9" s="37" t="s">
+      <c r="D9" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="E9" s="71" t="s">
+      <c r="E9" s="47" t="s">
         <v>143</v>
       </c>
-      <c r="F9" s="42"/>
-      <c r="G9" s="39" t="s">
+      <c r="F9" s="19"/>
+      <c r="G9" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="H9" s="38">
+      <c r="H9" s="15">
         <v>7</v>
       </c>
-      <c r="I9" s="38" t="s">
+      <c r="I9" s="15" t="s">
         <v>19</v>
       </c>
       <c r="J9" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="K9" s="40" t="s">
+      <c r="K9" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="L9" s="39" t="s">
+      <c r="L9" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="M9" s="41"/>
-      <c r="N9" s="41"/>
-      <c r="O9" s="42"/>
-      <c r="P9" s="42"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
       <c r="Q9" s="3">
         <v>8</v>
       </c>
-      <c r="R9" s="43" t="s">
+      <c r="R9" s="20" t="s">
         <v>138</v>
       </c>
       <c r="S9" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="T9" s="44" t="s">
+      <c r="T9" s="21" t="s">
         <v>140</v>
       </c>
       <c r="U9" s="3" t="s">
@@ -1921,54 +1923,54 @@
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="E10" s="55" t="s">
+      <c r="E10" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="F10" s="47"/>
-      <c r="G10" s="39" t="s">
+      <c r="F10" s="24"/>
+      <c r="G10" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="H10" s="38">
+      <c r="H10" s="15">
         <v>8</v>
       </c>
-      <c r="I10" s="48" t="s">
+      <c r="I10" s="25" t="s">
         <v>20</v>
       </c>
       <c r="J10" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="K10" s="49" t="s">
+      <c r="K10" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="L10" s="50" t="s">
+      <c r="L10" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="M10" s="51"/>
-      <c r="N10" s="51"/>
-      <c r="O10" s="47"/>
-      <c r="P10" s="47"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
       <c r="Q10" s="4">
         <v>8</v>
       </c>
-      <c r="R10" s="52" t="s">
+      <c r="R10" s="29" t="s">
         <v>138</v>
       </c>
       <c r="S10" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="T10" s="53" t="s">
+      <c r="T10" s="30" t="s">
         <v>142</v>
       </c>
       <c r="U10" s="4" t="s">
@@ -1976,113 +1978,113 @@
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="D11" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="E11" s="55" t="s">
+      <c r="E11" s="31" t="s">
         <v>145</v>
       </c>
-      <c r="F11" s="47"/>
-      <c r="G11" s="39" t="s">
+      <c r="F11" s="24"/>
+      <c r="G11" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="H11" s="38">
+      <c r="H11" s="15">
         <v>9</v>
       </c>
-      <c r="I11" s="48" t="s">
+      <c r="I11" s="25" t="s">
         <v>20</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="K11" s="49" t="s">
+      <c r="K11" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="L11" s="50" t="s">
+      <c r="L11" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="M11" s="51"/>
-      <c r="N11" s="51" t="s">
+      <c r="M11" s="28"/>
+      <c r="N11" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="O11" s="47"/>
-      <c r="P11" s="47"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
       <c r="Q11" s="3">
         <v>6</v>
       </c>
-      <c r="R11" s="43" t="s">
+      <c r="R11" s="20" t="s">
         <v>171</v>
       </c>
       <c r="S11" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="T11" s="44" t="s">
+      <c r="T11" s="21" t="s">
         <v>182</v>
       </c>
       <c r="U11" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="12" spans="1:21" s="70" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="57" t="s">
+    <row r="12" spans="1:21" s="46" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="C12" s="59" t="s">
+      <c r="C12" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="D12" s="57" t="s">
+      <c r="D12" s="33" t="s">
         <v>159</v>
       </c>
-      <c r="E12" s="60" t="s">
+      <c r="E12" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="F12" s="72"/>
-      <c r="G12" s="62" t="s">
+      <c r="F12" s="48"/>
+      <c r="G12" s="38" t="s">
         <v>147</v>
       </c>
-      <c r="H12" s="63">
+      <c r="H12" s="39">
         <v>10</v>
       </c>
-      <c r="I12" s="63" t="s">
+      <c r="I12" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="65" t="s">
+      <c r="J12" s="41" t="s">
         <v>196</v>
       </c>
-      <c r="K12" s="73" t="s">
+      <c r="K12" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="L12" s="74" t="s">
+      <c r="L12" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="M12" s="75"/>
-      <c r="N12" s="75" t="s">
+      <c r="M12" s="51"/>
+      <c r="N12" s="51" t="s">
         <v>121</v>
       </c>
-      <c r="O12" s="72"/>
-      <c r="P12" s="72"/>
+      <c r="O12" s="48"/>
+      <c r="P12" s="48"/>
       <c r="Q12" s="6">
         <v>6</v>
       </c>
-      <c r="R12" s="68" t="s">
+      <c r="R12" s="44" t="s">
         <v>171</v>
       </c>
       <c r="S12" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="T12" s="69" t="s">
+      <c r="T12" s="45" t="s">
         <v>179</v>
       </c>
       <c r="U12" s="6" t="s">
@@ -2090,54 +2092,54 @@
       </c>
     </row>
     <row r="13" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="E13" s="71"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="39" t="s">
+      <c r="E13" s="47"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="H13" s="38">
+      <c r="H13" s="15">
         <v>11</v>
       </c>
-      <c r="I13" s="38" t="s">
+      <c r="I13" s="15" t="s">
         <v>19</v>
       </c>
       <c r="J13" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="K13" s="40" t="s">
+      <c r="K13" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="L13" s="39" t="s">
+      <c r="L13" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="M13" s="41" t="s">
+      <c r="M13" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="N13" s="41"/>
-      <c r="O13" s="42"/>
-      <c r="P13" s="42"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
       <c r="Q13" s="3">
         <v>6</v>
       </c>
-      <c r="R13" s="43" t="s">
+      <c r="R13" s="20" t="s">
         <v>167</v>
       </c>
       <c r="S13" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="T13" s="44" t="s">
+      <c r="T13" s="21" t="s">
         <v>185</v>
       </c>
       <c r="U13" s="3" t="s">
@@ -2145,54 +2147,54 @@
       </c>
     </row>
     <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="D14" s="34" t="s">
+      <c r="D14" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="E14" s="55"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="39" t="s">
+      <c r="E14" s="31"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="H14" s="38">
+      <c r="H14" s="15">
         <v>12</v>
       </c>
-      <c r="I14" s="48" t="s">
+      <c r="I14" s="25" t="s">
         <v>20</v>
       </c>
       <c r="J14" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="K14" s="49" t="s">
+      <c r="K14" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="50" t="s">
+      <c r="L14" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="M14" s="51"/>
-      <c r="N14" s="51" t="s">
+      <c r="M14" s="28"/>
+      <c r="N14" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="O14" s="47"/>
-      <c r="P14" s="47"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="24"/>
       <c r="Q14" s="4">
         <v>6</v>
       </c>
-      <c r="R14" s="52" t="s">
+      <c r="R14" s="29" t="s">
         <v>171</v>
       </c>
       <c r="S14" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="T14" s="53" t="s">
+      <c r="T14" s="30" t="s">
         <v>186</v>
       </c>
       <c r="U14" s="4" t="s">
@@ -2200,54 +2202,54 @@
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="E15" s="55"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="39" t="s">
+      <c r="E15" s="31"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="H15" s="38">
+      <c r="H15" s="15">
         <v>13</v>
       </c>
-      <c r="I15" s="48" t="s">
+      <c r="I15" s="25" t="s">
         <v>20</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="K15" s="49" t="s">
+      <c r="K15" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="L15" s="50" t="s">
+      <c r="L15" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="51"/>
-      <c r="N15" s="51" t="s">
+      <c r="M15" s="28"/>
+      <c r="N15" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="O15" s="47"/>
-      <c r="P15" s="47"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="24"/>
       <c r="Q15" s="4">
         <v>6</v>
       </c>
-      <c r="R15" s="52" t="s">
+      <c r="R15" s="29" t="s">
         <v>171</v>
       </c>
       <c r="S15" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="T15" s="53" t="s">
+      <c r="T15" s="30" t="s">
         <v>187</v>
       </c>
       <c r="U15" s="4" t="s">
@@ -2255,111 +2257,111 @@
       </c>
     </row>
     <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C16" s="36" t="s">
+      <c r="C16" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="D16" s="34" t="s">
+      <c r="D16" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="E16" s="55"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="39" t="s">
+      <c r="E16" s="31"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="H16" s="38">
+      <c r="H16" s="15">
         <v>14</v>
       </c>
-      <c r="I16" s="48" t="s">
+      <c r="I16" s="25" t="s">
         <v>20</v>
       </c>
       <c r="J16" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="K16" s="49" t="s">
+      <c r="K16" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="L16" s="50" t="s">
+      <c r="L16" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="M16" s="51"/>
-      <c r="N16" s="51" t="s">
+      <c r="M16" s="28"/>
+      <c r="N16" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="O16" s="47"/>
-      <c r="P16" s="47"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24"/>
       <c r="Q16" s="3">
         <v>6</v>
       </c>
-      <c r="R16" s="43" t="s">
+      <c r="R16" s="20" t="s">
         <v>171</v>
       </c>
       <c r="S16" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="T16" s="44" t="s">
+      <c r="T16" s="21" t="s">
         <v>183</v>
       </c>
       <c r="U16" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="17" spans="1:21" s="70" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="57" t="s">
+    <row r="17" spans="1:21" s="46" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="C17" s="59" t="s">
+      <c r="C17" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="D17" s="57" t="s">
+      <c r="D17" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="E17" s="60" t="s">
+      <c r="E17" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="F17" s="72"/>
-      <c r="G17" s="62" t="s">
+      <c r="F17" s="48"/>
+      <c r="G17" s="38" t="s">
         <v>156</v>
       </c>
-      <c r="H17" s="63">
+      <c r="H17" s="39">
         <v>15</v>
       </c>
-      <c r="I17" s="63" t="s">
+      <c r="I17" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="65" t="s">
+      <c r="J17" s="41" t="s">
         <v>201</v>
       </c>
-      <c r="K17" s="73" t="s">
+      <c r="K17" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="L17" s="74" t="s">
+      <c r="L17" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="M17" s="75"/>
-      <c r="N17" s="75" t="s">
+      <c r="M17" s="51"/>
+      <c r="N17" s="51" t="s">
         <v>121</v>
       </c>
-      <c r="O17" s="72"/>
-      <c r="P17" s="72"/>
+      <c r="O17" s="48"/>
+      <c r="P17" s="48"/>
       <c r="Q17" s="5">
         <v>6</v>
       </c>
-      <c r="R17" s="76" t="s">
+      <c r="R17" s="52" t="s">
         <v>171</v>
       </c>
       <c r="S17" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="T17" s="77" t="s">
+      <c r="T17" s="53" t="s">
         <v>180</v>
       </c>
       <c r="U17" s="5" t="s">
@@ -2367,107 +2369,107 @@
       </c>
     </row>
     <row r="18" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C18" s="36" t="s">
+      <c r="C18" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="D18" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="E18" s="71"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="39" t="s">
+      <c r="E18" s="47"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="H18" s="38">
+      <c r="H18" s="15">
         <v>16</v>
       </c>
-      <c r="I18" s="38" t="s">
+      <c r="I18" s="15" t="s">
         <v>20</v>
       </c>
       <c r="J18" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="K18" s="40" t="s">
+      <c r="K18" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="L18" s="39" t="s">
+      <c r="L18" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="M18" s="41"/>
-      <c r="N18" s="41"/>
-      <c r="O18" s="42"/>
-      <c r="P18" s="42"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="19"/>
       <c r="Q18" s="3">
         <v>8</v>
       </c>
-      <c r="R18" s="43" t="s">
+      <c r="R18" s="20" t="s">
         <v>138</v>
       </c>
       <c r="S18" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="T18" s="44" t="s">
+      <c r="T18" s="21" t="s">
         <v>154</v>
       </c>
       <c r="U18" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="1:21" s="70" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="57" t="s">
+    <row r="19" spans="1:21" s="46" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="C19" s="59" t="s">
+      <c r="C19" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="D19" s="57" t="s">
+      <c r="D19" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="E19" s="78"/>
-      <c r="F19" s="72"/>
-      <c r="G19" s="62" t="s">
+      <c r="E19" s="54"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="38" t="s">
         <v>161</v>
       </c>
-      <c r="H19" s="63">
+      <c r="H19" s="39">
         <v>17</v>
       </c>
-      <c r="I19" s="63" t="s">
+      <c r="I19" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="65" t="s">
+      <c r="J19" s="41" t="s">
         <v>203</v>
       </c>
-      <c r="K19" s="73" t="s">
+      <c r="K19" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="L19" s="74" t="s">
+      <c r="L19" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="M19" s="75"/>
-      <c r="N19" s="75" t="s">
+      <c r="M19" s="51"/>
+      <c r="N19" s="51" t="s">
         <v>120</v>
       </c>
-      <c r="O19" s="72"/>
-      <c r="P19" s="72"/>
+      <c r="O19" s="48"/>
+      <c r="P19" s="48"/>
       <c r="Q19" s="6">
         <v>6</v>
       </c>
-      <c r="R19" s="68" t="s">
+      <c r="R19" s="44" t="s">
         <v>171</v>
       </c>
       <c r="S19" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="T19" s="69" t="s">
+      <c r="T19" s="45" t="s">
         <v>188</v>
       </c>
       <c r="U19" s="6" t="s">
@@ -2475,97 +2477,97 @@
       </c>
     </row>
     <row r="20" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="D20" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="E20" s="71"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="39" t="s">
+      <c r="E20" s="47"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H20" s="38">
+      <c r="H20" s="15">
         <v>18</v>
       </c>
-      <c r="I20" s="38" t="s">
+      <c r="I20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="J20" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="K20" s="40" t="s">
+      <c r="K20" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="L20" s="39" t="s">
+      <c r="L20" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="M20" s="41"/>
-      <c r="N20" s="41"/>
-      <c r="O20" s="42"/>
-      <c r="P20" s="42"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
       <c r="Q20" s="3"/>
-      <c r="R20" s="43"/>
+      <c r="R20" s="20"/>
       <c r="S20" s="3"/>
-      <c r="T20" s="44"/>
+      <c r="T20" s="21"/>
       <c r="U20" s="3"/>
     </row>
     <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="C21" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="D21" s="34" t="s">
+      <c r="D21" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="E21" s="55"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="39" t="s">
+      <c r="E21" s="31"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="H21" s="38">
+      <c r="H21" s="15">
         <v>19</v>
       </c>
-      <c r="I21" s="48" t="s">
+      <c r="I21" s="25" t="s">
         <v>20</v>
       </c>
       <c r="J21" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="K21" s="49" t="s">
+      <c r="K21" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="L21" s="50" t="s">
+      <c r="L21" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="M21" s="51"/>
-      <c r="N21" s="51" t="s">
+      <c r="M21" s="28"/>
+      <c r="N21" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="O21" s="47"/>
-      <c r="P21" s="47"/>
+      <c r="O21" s="24"/>
+      <c r="P21" s="24"/>
       <c r="Q21" s="4">
         <v>6</v>
       </c>
-      <c r="R21" s="52" t="s">
+      <c r="R21" s="29" t="s">
         <v>171</v>
       </c>
       <c r="S21" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="T21" s="53" t="s">
+      <c r="T21" s="30" t="s">
         <v>184</v>
       </c>
       <c r="U21" s="4" t="s">
@@ -2573,54 +2575,54 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C22" s="36" t="s">
+      <c r="C22" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="D22" s="34" t="s">
+      <c r="D22" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="E22" s="55"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="39" t="s">
+      <c r="E22" s="31"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="H22" s="38">
+      <c r="H22" s="15">
         <v>20</v>
       </c>
-      <c r="I22" s="48" t="s">
+      <c r="I22" s="25" t="s">
         <v>20</v>
       </c>
       <c r="J22" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="K22" s="49" t="s">
+      <c r="K22" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="L22" s="50" t="s">
+      <c r="L22" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="M22" s="51"/>
-      <c r="N22" s="51" t="s">
+      <c r="M22" s="28"/>
+      <c r="N22" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="O22" s="47"/>
-      <c r="P22" s="47"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="24"/>
       <c r="Q22" s="4">
         <v>6</v>
       </c>
-      <c r="R22" s="52" t="s">
+      <c r="R22" s="29" t="s">
         <v>171</v>
       </c>
       <c r="S22" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="T22" s="53" t="s">
+      <c r="T22" s="30" t="s">
         <v>181</v>
       </c>
       <c r="U22" s="4" t="s">
@@ -2628,1130 +2630,1130 @@
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="34"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="48"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="25"/>
       <c r="J23" s="8"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="50"/>
-      <c r="M23" s="51"/>
-      <c r="N23" s="51"/>
-      <c r="O23" s="47"/>
-      <c r="P23" s="47"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="28"/>
+      <c r="N23" s="28"/>
+      <c r="O23" s="24"/>
+      <c r="P23" s="24"/>
       <c r="Q23" s="3"/>
-      <c r="R23" s="43"/>
+      <c r="R23" s="20"/>
       <c r="S23" s="3"/>
-      <c r="T23" s="44"/>
+      <c r="T23" s="21"/>
       <c r="U23" s="3"/>
     </row>
     <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="34"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="48"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="25"/>
       <c r="J24" s="8"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="50"/>
-      <c r="M24" s="51"/>
-      <c r="N24" s="51"/>
-      <c r="O24" s="47"/>
-      <c r="P24" s="47"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="24"/>
+      <c r="P24" s="24"/>
       <c r="Q24" s="3"/>
-      <c r="R24" s="43"/>
+      <c r="R24" s="20"/>
       <c r="S24" s="3"/>
-      <c r="T24" s="44"/>
+      <c r="T24" s="21"/>
       <c r="U24" s="3"/>
     </row>
     <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="34"/>
-      <c r="B25" s="35"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="47"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="48"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="25"/>
       <c r="J25" s="8"/>
-      <c r="K25" s="49"/>
-      <c r="L25" s="50"/>
-      <c r="M25" s="51"/>
-      <c r="N25" s="51"/>
-      <c r="O25" s="47"/>
-      <c r="P25" s="47"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="27"/>
+      <c r="M25" s="28"/>
+      <c r="N25" s="28"/>
+      <c r="O25" s="24"/>
+      <c r="P25" s="24"/>
       <c r="Q25" s="4"/>
-      <c r="R25" s="52"/>
+      <c r="R25" s="29"/>
       <c r="S25" s="4"/>
-      <c r="T25" s="53"/>
+      <c r="T25" s="30"/>
       <c r="U25" s="4"/>
     </row>
     <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="48"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="25"/>
       <c r="J26" s="8"/>
-      <c r="K26" s="49"/>
-      <c r="L26" s="50"/>
-      <c r="M26" s="51"/>
-      <c r="N26" s="51"/>
-      <c r="O26" s="47"/>
-      <c r="P26" s="47"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="27"/>
+      <c r="M26" s="28"/>
+      <c r="N26" s="28"/>
+      <c r="O26" s="24"/>
+      <c r="P26" s="24"/>
       <c r="Q26" s="4"/>
-      <c r="R26" s="52"/>
+      <c r="R26" s="29"/>
       <c r="S26" s="4"/>
-      <c r="T26" s="53"/>
+      <c r="T26" s="30"/>
       <c r="U26" s="4"/>
     </row>
     <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
-      <c r="B27" s="35"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="48"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="25"/>
       <c r="J27" s="8"/>
-      <c r="K27" s="49"/>
-      <c r="L27" s="50"/>
-      <c r="M27" s="51"/>
-      <c r="N27" s="51"/>
-      <c r="O27" s="47"/>
-      <c r="P27" s="47"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="27"/>
+      <c r="M27" s="28"/>
+      <c r="N27" s="28"/>
+      <c r="O27" s="24"/>
+      <c r="P27" s="24"/>
       <c r="Q27" s="4"/>
-      <c r="R27" s="52"/>
+      <c r="R27" s="29"/>
       <c r="S27" s="4"/>
-      <c r="T27" s="53"/>
+      <c r="T27" s="30"/>
       <c r="U27" s="4"/>
     </row>
     <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
-      <c r="B28" s="35"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="55"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="48"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="25"/>
       <c r="J28" s="8"/>
-      <c r="K28" s="49"/>
-      <c r="L28" s="50"/>
-      <c r="M28" s="51"/>
-      <c r="N28" s="51"/>
-      <c r="O28" s="47"/>
-      <c r="P28" s="47"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="27"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="24"/>
+      <c r="P28" s="24"/>
       <c r="Q28" s="4"/>
-      <c r="R28" s="52"/>
+      <c r="R28" s="29"/>
       <c r="S28" s="4"/>
-      <c r="T28" s="53"/>
+      <c r="T28" s="30"/>
       <c r="U28" s="4"/>
     </row>
     <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="34"/>
-      <c r="B29" s="35"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="48"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="25"/>
       <c r="J29" s="8"/>
-      <c r="K29" s="49"/>
-      <c r="L29" s="50"/>
-      <c r="M29" s="51"/>
-      <c r="N29" s="51"/>
-      <c r="O29" s="47"/>
-      <c r="P29" s="47"/>
+      <c r="K29" s="26"/>
+      <c r="L29" s="27"/>
+      <c r="M29" s="28"/>
+      <c r="N29" s="28"/>
+      <c r="O29" s="24"/>
+      <c r="P29" s="24"/>
       <c r="Q29" s="4"/>
-      <c r="R29" s="52"/>
+      <c r="R29" s="29"/>
       <c r="S29" s="4"/>
-      <c r="T29" s="53"/>
+      <c r="T29" s="30"/>
       <c r="U29" s="4"/>
     </row>
     <row r="30" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="34"/>
-      <c r="B30" s="35"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="55"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="48"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="25"/>
       <c r="J30" s="8"/>
-      <c r="K30" s="49"/>
-      <c r="L30" s="50"/>
-      <c r="M30" s="51"/>
-      <c r="N30" s="51"/>
-      <c r="O30" s="47"/>
-      <c r="P30" s="47"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="27"/>
+      <c r="M30" s="28"/>
+      <c r="N30" s="28"/>
+      <c r="O30" s="24"/>
+      <c r="P30" s="24"/>
       <c r="Q30" s="4"/>
-      <c r="R30" s="52"/>
+      <c r="R30" s="29"/>
       <c r="S30" s="4"/>
-      <c r="T30" s="53"/>
+      <c r="T30" s="30"/>
       <c r="U30" s="4"/>
     </row>
     <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="34"/>
-      <c r="B31" s="35"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="55"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="48"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="25"/>
       <c r="J31" s="8"/>
-      <c r="K31" s="49"/>
-      <c r="L31" s="50"/>
-      <c r="M31" s="51"/>
-      <c r="N31" s="51"/>
-      <c r="O31" s="47"/>
-      <c r="P31" s="47"/>
+      <c r="K31" s="26"/>
+      <c r="L31" s="27"/>
+      <c r="M31" s="28"/>
+      <c r="N31" s="28"/>
+      <c r="O31" s="24"/>
+      <c r="P31" s="24"/>
       <c r="Q31" s="4"/>
-      <c r="R31" s="52"/>
+      <c r="R31" s="29"/>
       <c r="S31" s="4"/>
-      <c r="T31" s="53"/>
+      <c r="T31" s="30"/>
       <c r="U31" s="4"/>
     </row>
     <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="79"/>
-      <c r="B32" s="46"/>
-      <c r="C32" s="80"/>
-      <c r="D32" s="81"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="82"/>
-      <c r="H32" s="47"/>
-      <c r="I32" s="48"/>
+      <c r="A32" s="55"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="25"/>
       <c r="J32" s="8"/>
-      <c r="K32" s="49"/>
-      <c r="L32" s="50"/>
-      <c r="M32" s="51"/>
-      <c r="N32" s="51"/>
-      <c r="O32" s="47"/>
-      <c r="P32" s="47"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="27"/>
+      <c r="M32" s="28"/>
+      <c r="N32" s="28"/>
+      <c r="O32" s="24"/>
+      <c r="P32" s="24"/>
       <c r="Q32" s="4"/>
-      <c r="R32" s="52"/>
+      <c r="R32" s="29"/>
       <c r="S32" s="4"/>
-      <c r="T32" s="53"/>
+      <c r="T32" s="30"/>
       <c r="U32" s="4"/>
     </row>
     <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="79"/>
-      <c r="B33" s="46"/>
-      <c r="C33" s="80"/>
-      <c r="D33" s="81"/>
-      <c r="E33" s="46"/>
-      <c r="F33" s="47"/>
-      <c r="G33" s="82"/>
-      <c r="H33" s="47"/>
-      <c r="I33" s="48"/>
+      <c r="A33" s="55"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="58"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="25"/>
       <c r="J33" s="8"/>
-      <c r="K33" s="49"/>
-      <c r="L33" s="50"/>
-      <c r="M33" s="51"/>
-      <c r="N33" s="51"/>
-      <c r="O33" s="47"/>
-      <c r="P33" s="47"/>
+      <c r="K33" s="26"/>
+      <c r="L33" s="27"/>
+      <c r="M33" s="28"/>
+      <c r="N33" s="28"/>
+      <c r="O33" s="24"/>
+      <c r="P33" s="24"/>
       <c r="Q33" s="4"/>
-      <c r="R33" s="52"/>
+      <c r="R33" s="29"/>
       <c r="S33" s="4"/>
-      <c r="T33" s="53"/>
+      <c r="T33" s="30"/>
       <c r="U33" s="4"/>
     </row>
     <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="79"/>
-      <c r="B34" s="46"/>
-      <c r="C34" s="80"/>
-      <c r="D34" s="81"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="47"/>
-      <c r="G34" s="82"/>
-      <c r="H34" s="47"/>
-      <c r="I34" s="48"/>
+      <c r="A34" s="55"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="25"/>
       <c r="J34" s="8"/>
-      <c r="K34" s="49"/>
-      <c r="L34" s="50"/>
-      <c r="M34" s="51"/>
-      <c r="N34" s="51"/>
-      <c r="O34" s="47"/>
-      <c r="P34" s="47"/>
+      <c r="K34" s="26"/>
+      <c r="L34" s="27"/>
+      <c r="M34" s="28"/>
+      <c r="N34" s="28"/>
+      <c r="O34" s="24"/>
+      <c r="P34" s="24"/>
       <c r="Q34" s="4"/>
-      <c r="R34" s="52"/>
+      <c r="R34" s="29"/>
       <c r="S34" s="4"/>
-      <c r="T34" s="53"/>
+      <c r="T34" s="30"/>
       <c r="U34" s="4"/>
     </row>
     <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="79"/>
-      <c r="B35" s="46"/>
-      <c r="C35" s="80"/>
-      <c r="D35" s="81"/>
-      <c r="E35" s="46"/>
-      <c r="F35" s="47"/>
-      <c r="G35" s="82"/>
-      <c r="H35" s="47"/>
-      <c r="I35" s="48"/>
+      <c r="A35" s="55"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="58"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="25"/>
       <c r="J35" s="8"/>
-      <c r="K35" s="49"/>
-      <c r="L35" s="50"/>
-      <c r="M35" s="51"/>
-      <c r="N35" s="51"/>
-      <c r="O35" s="47"/>
-      <c r="P35" s="47"/>
+      <c r="K35" s="26"/>
+      <c r="L35" s="27"/>
+      <c r="M35" s="28"/>
+      <c r="N35" s="28"/>
+      <c r="O35" s="24"/>
+      <c r="P35" s="24"/>
       <c r="Q35" s="4"/>
-      <c r="R35" s="52"/>
+      <c r="R35" s="29"/>
       <c r="S35" s="4"/>
-      <c r="T35" s="53"/>
+      <c r="T35" s="30"/>
       <c r="U35" s="4"/>
     </row>
     <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="79"/>
-      <c r="B36" s="46"/>
-      <c r="C36" s="80"/>
-      <c r="D36" s="81"/>
-      <c r="E36" s="46"/>
-      <c r="F36" s="47"/>
-      <c r="G36" s="82"/>
-      <c r="H36" s="47"/>
-      <c r="I36" s="48"/>
+      <c r="A36" s="55"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="58"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="25"/>
       <c r="J36" s="8"/>
-      <c r="K36" s="49"/>
-      <c r="L36" s="50"/>
-      <c r="M36" s="51"/>
-      <c r="N36" s="51"/>
-      <c r="O36" s="47"/>
-      <c r="P36" s="47"/>
+      <c r="K36" s="26"/>
+      <c r="L36" s="27"/>
+      <c r="M36" s="28"/>
+      <c r="N36" s="28"/>
+      <c r="O36" s="24"/>
+      <c r="P36" s="24"/>
       <c r="Q36" s="4"/>
-      <c r="R36" s="52"/>
+      <c r="R36" s="29"/>
       <c r="S36" s="4"/>
-      <c r="T36" s="53"/>
+      <c r="T36" s="30"/>
       <c r="U36" s="4"/>
     </row>
     <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="79"/>
-      <c r="B37" s="46"/>
-      <c r="C37" s="80"/>
-      <c r="D37" s="81"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="47"/>
-      <c r="G37" s="82"/>
-      <c r="H37" s="47"/>
-      <c r="I37" s="48"/>
+      <c r="A37" s="55"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="56"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="58"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="25"/>
       <c r="J37" s="8"/>
-      <c r="K37" s="49"/>
-      <c r="L37" s="50"/>
-      <c r="M37" s="51"/>
-      <c r="N37" s="51"/>
-      <c r="O37" s="47"/>
-      <c r="P37" s="47"/>
+      <c r="K37" s="26"/>
+      <c r="L37" s="27"/>
+      <c r="M37" s="28"/>
+      <c r="N37" s="28"/>
+      <c r="O37" s="24"/>
+      <c r="P37" s="24"/>
       <c r="Q37" s="4"/>
-      <c r="R37" s="52"/>
+      <c r="R37" s="29"/>
       <c r="S37" s="4"/>
-      <c r="T37" s="53"/>
+      <c r="T37" s="30"/>
       <c r="U37" s="4"/>
     </row>
     <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="79"/>
-      <c r="B38" s="46"/>
-      <c r="C38" s="80"/>
-      <c r="D38" s="81"/>
-      <c r="E38" s="46"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="82"/>
-      <c r="H38" s="47"/>
-      <c r="I38" s="48"/>
+      <c r="A38" s="55"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="58"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="25"/>
       <c r="J38" s="8"/>
-      <c r="K38" s="49"/>
-      <c r="L38" s="50"/>
-      <c r="M38" s="51"/>
-      <c r="N38" s="51"/>
-      <c r="O38" s="47"/>
-      <c r="P38" s="47"/>
+      <c r="K38" s="26"/>
+      <c r="L38" s="27"/>
+      <c r="M38" s="28"/>
+      <c r="N38" s="28"/>
+      <c r="O38" s="24"/>
+      <c r="P38" s="24"/>
       <c r="Q38" s="4"/>
-      <c r="R38" s="52"/>
+      <c r="R38" s="29"/>
       <c r="S38" s="4"/>
-      <c r="T38" s="53"/>
+      <c r="T38" s="30"/>
       <c r="U38" s="4"/>
     </row>
     <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="79"/>
-      <c r="B39" s="46"/>
-      <c r="C39" s="80"/>
-      <c r="D39" s="81"/>
-      <c r="E39" s="46"/>
-      <c r="F39" s="47"/>
-      <c r="G39" s="82"/>
-      <c r="H39" s="47"/>
-      <c r="I39" s="48"/>
+      <c r="A39" s="55"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="58"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="25"/>
       <c r="J39" s="8"/>
-      <c r="K39" s="49"/>
-      <c r="L39" s="50"/>
-      <c r="M39" s="51"/>
-      <c r="N39" s="51"/>
-      <c r="O39" s="47"/>
-      <c r="P39" s="47"/>
+      <c r="K39" s="26"/>
+      <c r="L39" s="27"/>
+      <c r="M39" s="28"/>
+      <c r="N39" s="28"/>
+      <c r="O39" s="24"/>
+      <c r="P39" s="24"/>
       <c r="Q39" s="4"/>
-      <c r="R39" s="52"/>
+      <c r="R39" s="29"/>
       <c r="S39" s="4"/>
-      <c r="T39" s="53"/>
+      <c r="T39" s="30"/>
       <c r="U39" s="4"/>
     </row>
     <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="79"/>
-      <c r="B40" s="46"/>
-      <c r="C40" s="80"/>
-      <c r="D40" s="81"/>
-      <c r="E40" s="46"/>
-      <c r="F40" s="47"/>
-      <c r="G40" s="82"/>
-      <c r="H40" s="47"/>
-      <c r="I40" s="48"/>
+      <c r="A40" s="55"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="56"/>
+      <c r="D40" s="57"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="58"/>
+      <c r="H40" s="24"/>
+      <c r="I40" s="25"/>
       <c r="J40" s="8"/>
-      <c r="K40" s="49"/>
-      <c r="L40" s="50"/>
-      <c r="M40" s="51"/>
-      <c r="N40" s="51"/>
-      <c r="O40" s="47"/>
-      <c r="P40" s="47"/>
+      <c r="K40" s="26"/>
+      <c r="L40" s="27"/>
+      <c r="M40" s="28"/>
+      <c r="N40" s="28"/>
+      <c r="O40" s="24"/>
+      <c r="P40" s="24"/>
       <c r="Q40" s="4"/>
-      <c r="R40" s="52"/>
+      <c r="R40" s="29"/>
       <c r="S40" s="4"/>
-      <c r="T40" s="53"/>
+      <c r="T40" s="30"/>
       <c r="U40" s="4"/>
     </row>
     <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="79"/>
-      <c r="B41" s="46"/>
-      <c r="C41" s="80"/>
-      <c r="D41" s="81"/>
-      <c r="E41" s="46"/>
-      <c r="F41" s="47"/>
-      <c r="G41" s="82"/>
-      <c r="H41" s="47"/>
-      <c r="I41" s="48"/>
+      <c r="A41" s="55"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="56"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="58"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="25"/>
       <c r="J41" s="8"/>
-      <c r="K41" s="49"/>
-      <c r="L41" s="50"/>
-      <c r="M41" s="51"/>
-      <c r="N41" s="51"/>
-      <c r="O41" s="47"/>
-      <c r="P41" s="47"/>
+      <c r="K41" s="26"/>
+      <c r="L41" s="27"/>
+      <c r="M41" s="28"/>
+      <c r="N41" s="28"/>
+      <c r="O41" s="24"/>
+      <c r="P41" s="24"/>
       <c r="Q41" s="4"/>
-      <c r="R41" s="52"/>
+      <c r="R41" s="29"/>
       <c r="S41" s="4"/>
-      <c r="T41" s="53"/>
+      <c r="T41" s="30"/>
       <c r="U41" s="4"/>
     </row>
     <row r="42" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="79"/>
-      <c r="B42" s="46"/>
-      <c r="C42" s="80"/>
-      <c r="D42" s="81"/>
-      <c r="E42" s="46"/>
-      <c r="F42" s="47"/>
-      <c r="G42" s="82"/>
-      <c r="H42" s="47"/>
-      <c r="I42" s="48"/>
+      <c r="A42" s="55"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="56"/>
+      <c r="D42" s="57"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="58"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="25"/>
       <c r="J42" s="8"/>
-      <c r="K42" s="49"/>
-      <c r="L42" s="50"/>
-      <c r="M42" s="51"/>
-      <c r="N42" s="51"/>
-      <c r="O42" s="47"/>
-      <c r="P42" s="47"/>
+      <c r="K42" s="26"/>
+      <c r="L42" s="27"/>
+      <c r="M42" s="28"/>
+      <c r="N42" s="28"/>
+      <c r="O42" s="24"/>
+      <c r="P42" s="24"/>
       <c r="Q42" s="4"/>
-      <c r="R42" s="52"/>
+      <c r="R42" s="29"/>
       <c r="S42" s="4"/>
-      <c r="T42" s="53"/>
+      <c r="T42" s="30"/>
       <c r="U42" s="4"/>
     </row>
     <row r="43" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="79"/>
-      <c r="B43" s="46"/>
-      <c r="C43" s="80"/>
-      <c r="D43" s="81"/>
-      <c r="E43" s="46"/>
-      <c r="F43" s="47"/>
-      <c r="G43" s="82"/>
-      <c r="H43" s="47"/>
-      <c r="I43" s="48"/>
+      <c r="A43" s="55"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="56"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="23"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="58"/>
+      <c r="H43" s="24"/>
+      <c r="I43" s="25"/>
       <c r="J43" s="8"/>
-      <c r="K43" s="49"/>
-      <c r="L43" s="50"/>
-      <c r="M43" s="51"/>
-      <c r="N43" s="51"/>
-      <c r="O43" s="47"/>
-      <c r="P43" s="47"/>
+      <c r="K43" s="26"/>
+      <c r="L43" s="27"/>
+      <c r="M43" s="28"/>
+      <c r="N43" s="28"/>
+      <c r="O43" s="24"/>
+      <c r="P43" s="24"/>
       <c r="Q43" s="4"/>
-      <c r="R43" s="52"/>
+      <c r="R43" s="29"/>
       <c r="S43" s="4"/>
-      <c r="T43" s="53"/>
+      <c r="T43" s="30"/>
       <c r="U43" s="4"/>
     </row>
     <row r="44" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="79"/>
-      <c r="B44" s="46"/>
-      <c r="C44" s="80"/>
-      <c r="D44" s="81"/>
-      <c r="E44" s="46"/>
-      <c r="F44" s="47"/>
-      <c r="G44" s="82"/>
-      <c r="H44" s="47"/>
-      <c r="I44" s="48"/>
+      <c r="A44" s="55"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="56"/>
+      <c r="D44" s="57"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="58"/>
+      <c r="H44" s="24"/>
+      <c r="I44" s="25"/>
       <c r="J44" s="8"/>
-      <c r="K44" s="49"/>
-      <c r="L44" s="50"/>
-      <c r="M44" s="51"/>
-      <c r="N44" s="51"/>
-      <c r="O44" s="47"/>
-      <c r="P44" s="47"/>
+      <c r="K44" s="26"/>
+      <c r="L44" s="27"/>
+      <c r="M44" s="28"/>
+      <c r="N44" s="28"/>
+      <c r="O44" s="24"/>
+      <c r="P44" s="24"/>
       <c r="Q44" s="4"/>
-      <c r="R44" s="52"/>
+      <c r="R44" s="29"/>
       <c r="S44" s="4"/>
-      <c r="T44" s="53"/>
+      <c r="T44" s="30"/>
       <c r="U44" s="4"/>
     </row>
     <row r="45" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="79"/>
-      <c r="B45" s="46"/>
-      <c r="C45" s="80"/>
-      <c r="D45" s="81"/>
-      <c r="E45" s="46"/>
-      <c r="F45" s="47"/>
-      <c r="G45" s="82"/>
-      <c r="H45" s="47"/>
-      <c r="I45" s="48"/>
+      <c r="A45" s="55"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="56"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="58"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="25"/>
       <c r="J45" s="8"/>
-      <c r="K45" s="49"/>
-      <c r="L45" s="50"/>
-      <c r="M45" s="51"/>
-      <c r="N45" s="51"/>
-      <c r="O45" s="47"/>
-      <c r="P45" s="47"/>
+      <c r="K45" s="26"/>
+      <c r="L45" s="27"/>
+      <c r="M45" s="28"/>
+      <c r="N45" s="28"/>
+      <c r="O45" s="24"/>
+      <c r="P45" s="24"/>
       <c r="Q45" s="4"/>
-      <c r="R45" s="52"/>
+      <c r="R45" s="29"/>
       <c r="S45" s="4"/>
-      <c r="T45" s="53"/>
+      <c r="T45" s="30"/>
       <c r="U45" s="4"/>
     </row>
     <row r="46" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="79"/>
-      <c r="B46" s="46"/>
-      <c r="C46" s="80"/>
-      <c r="D46" s="81"/>
-      <c r="E46" s="46"/>
-      <c r="F46" s="47"/>
-      <c r="G46" s="82"/>
-      <c r="H46" s="47"/>
-      <c r="I46" s="48"/>
+      <c r="A46" s="55"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="56"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="58"/>
+      <c r="H46" s="24"/>
+      <c r="I46" s="25"/>
       <c r="J46" s="8"/>
-      <c r="K46" s="49"/>
-      <c r="L46" s="50"/>
-      <c r="M46" s="51"/>
-      <c r="N46" s="51"/>
-      <c r="O46" s="47"/>
-      <c r="P46" s="47"/>
+      <c r="K46" s="26"/>
+      <c r="L46" s="27"/>
+      <c r="M46" s="28"/>
+      <c r="N46" s="28"/>
+      <c r="O46" s="24"/>
+      <c r="P46" s="24"/>
       <c r="Q46" s="4"/>
-      <c r="R46" s="52"/>
+      <c r="R46" s="29"/>
       <c r="S46" s="4"/>
-      <c r="T46" s="53"/>
+      <c r="T46" s="30"/>
       <c r="U46" s="4"/>
     </row>
     <row r="47" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="79"/>
-      <c r="B47" s="46"/>
-      <c r="C47" s="80"/>
-      <c r="D47" s="81"/>
-      <c r="E47" s="46"/>
-      <c r="F47" s="47"/>
-      <c r="G47" s="82"/>
-      <c r="H47" s="47"/>
-      <c r="I47" s="48"/>
+      <c r="A47" s="55"/>
+      <c r="B47" s="23"/>
+      <c r="C47" s="56"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="58"/>
+      <c r="H47" s="24"/>
+      <c r="I47" s="25"/>
       <c r="J47" s="8"/>
-      <c r="K47" s="49"/>
-      <c r="L47" s="50"/>
-      <c r="M47" s="51"/>
-      <c r="N47" s="51"/>
-      <c r="O47" s="47"/>
-      <c r="P47" s="47"/>
+      <c r="K47" s="26"/>
+      <c r="L47" s="27"/>
+      <c r="M47" s="28"/>
+      <c r="N47" s="28"/>
+      <c r="O47" s="24"/>
+      <c r="P47" s="24"/>
       <c r="Q47" s="4"/>
-      <c r="R47" s="52"/>
+      <c r="R47" s="29"/>
       <c r="S47" s="4"/>
-      <c r="T47" s="53"/>
+      <c r="T47" s="30"/>
       <c r="U47" s="4"/>
     </row>
     <row r="48" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="79"/>
-      <c r="B48" s="46"/>
-      <c r="C48" s="80"/>
-      <c r="D48" s="81"/>
-      <c r="E48" s="46"/>
-      <c r="F48" s="47"/>
-      <c r="G48" s="82"/>
-      <c r="H48" s="47"/>
-      <c r="I48" s="48"/>
+      <c r="A48" s="55"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="56"/>
+      <c r="D48" s="57"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="58"/>
+      <c r="H48" s="24"/>
+      <c r="I48" s="25"/>
       <c r="J48" s="8"/>
-      <c r="K48" s="49"/>
-      <c r="L48" s="50"/>
-      <c r="M48" s="51"/>
-      <c r="N48" s="51"/>
-      <c r="O48" s="47"/>
-      <c r="P48" s="47"/>
+      <c r="K48" s="26"/>
+      <c r="L48" s="27"/>
+      <c r="M48" s="28"/>
+      <c r="N48" s="28"/>
+      <c r="O48" s="24"/>
+      <c r="P48" s="24"/>
       <c r="Q48" s="4"/>
-      <c r="R48" s="52"/>
+      <c r="R48" s="29"/>
       <c r="S48" s="4"/>
-      <c r="T48" s="53"/>
+      <c r="T48" s="30"/>
       <c r="U48" s="4"/>
     </row>
     <row r="49" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="79"/>
-      <c r="B49" s="46"/>
-      <c r="C49" s="80"/>
-      <c r="D49" s="81"/>
-      <c r="E49" s="46"/>
-      <c r="F49" s="47"/>
-      <c r="G49" s="82"/>
-      <c r="H49" s="47"/>
-      <c r="I49" s="48"/>
+      <c r="A49" s="55"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="56"/>
+      <c r="D49" s="57"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="58"/>
+      <c r="H49" s="24"/>
+      <c r="I49" s="25"/>
       <c r="J49" s="8"/>
-      <c r="K49" s="49"/>
-      <c r="L49" s="50"/>
-      <c r="M49" s="51"/>
-      <c r="N49" s="51"/>
-      <c r="O49" s="47"/>
-      <c r="P49" s="47"/>
+      <c r="K49" s="26"/>
+      <c r="L49" s="27"/>
+      <c r="M49" s="28"/>
+      <c r="N49" s="28"/>
+      <c r="O49" s="24"/>
+      <c r="P49" s="24"/>
       <c r="Q49" s="4"/>
-      <c r="R49" s="52"/>
+      <c r="R49" s="29"/>
       <c r="S49" s="4"/>
-      <c r="T49" s="53"/>
+      <c r="T49" s="30"/>
       <c r="U49" s="4"/>
     </row>
     <row r="50" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="79"/>
-      <c r="B50" s="46"/>
-      <c r="C50" s="80"/>
-      <c r="D50" s="81"/>
-      <c r="E50" s="46"/>
-      <c r="F50" s="47"/>
-      <c r="G50" s="82"/>
-      <c r="H50" s="47"/>
-      <c r="I50" s="48"/>
+      <c r="A50" s="55"/>
+      <c r="B50" s="23"/>
+      <c r="C50" s="56"/>
+      <c r="D50" s="57"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="58"/>
+      <c r="H50" s="24"/>
+      <c r="I50" s="25"/>
       <c r="J50" s="8"/>
-      <c r="K50" s="49"/>
-      <c r="L50" s="50"/>
-      <c r="M50" s="51"/>
-      <c r="N50" s="51"/>
-      <c r="O50" s="47"/>
-      <c r="P50" s="47"/>
+      <c r="K50" s="26"/>
+      <c r="L50" s="27"/>
+      <c r="M50" s="28"/>
+      <c r="N50" s="28"/>
+      <c r="O50" s="24"/>
+      <c r="P50" s="24"/>
       <c r="Q50" s="4"/>
-      <c r="R50" s="52"/>
+      <c r="R50" s="29"/>
       <c r="S50" s="4"/>
-      <c r="T50" s="53"/>
+      <c r="T50" s="30"/>
       <c r="U50" s="4"/>
     </row>
     <row r="51" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="79"/>
-      <c r="B51" s="46"/>
-      <c r="C51" s="80"/>
-      <c r="D51" s="81"/>
-      <c r="E51" s="46"/>
-      <c r="F51" s="47"/>
-      <c r="G51" s="82"/>
-      <c r="H51" s="47"/>
-      <c r="I51" s="48"/>
+      <c r="A51" s="55"/>
+      <c r="B51" s="23"/>
+      <c r="C51" s="56"/>
+      <c r="D51" s="57"/>
+      <c r="E51" s="23"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="58"/>
+      <c r="H51" s="24"/>
+      <c r="I51" s="25"/>
       <c r="J51" s="8"/>
-      <c r="K51" s="49"/>
-      <c r="L51" s="50"/>
-      <c r="M51" s="51"/>
-      <c r="N51" s="51"/>
-      <c r="O51" s="47"/>
-      <c r="P51" s="47"/>
+      <c r="K51" s="26"/>
+      <c r="L51" s="27"/>
+      <c r="M51" s="28"/>
+      <c r="N51" s="28"/>
+      <c r="O51" s="24"/>
+      <c r="P51" s="24"/>
       <c r="Q51" s="4"/>
-      <c r="R51" s="52"/>
+      <c r="R51" s="29"/>
       <c r="S51" s="4"/>
-      <c r="T51" s="53"/>
+      <c r="T51" s="30"/>
       <c r="U51" s="4"/>
     </row>
     <row r="52" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="79"/>
-      <c r="B52" s="46"/>
-      <c r="C52" s="80"/>
-      <c r="D52" s="81"/>
-      <c r="E52" s="46"/>
-      <c r="F52" s="47"/>
-      <c r="G52" s="82"/>
-      <c r="H52" s="47"/>
-      <c r="I52" s="48"/>
+      <c r="A52" s="55"/>
+      <c r="B52" s="23"/>
+      <c r="C52" s="56"/>
+      <c r="D52" s="57"/>
+      <c r="E52" s="23"/>
+      <c r="F52" s="24"/>
+      <c r="G52" s="58"/>
+      <c r="H52" s="24"/>
+      <c r="I52" s="25"/>
       <c r="J52" s="8"/>
-      <c r="K52" s="49"/>
-      <c r="L52" s="50"/>
-      <c r="M52" s="51"/>
-      <c r="N52" s="51"/>
-      <c r="O52" s="47"/>
-      <c r="P52" s="47"/>
+      <c r="K52" s="26"/>
+      <c r="L52" s="27"/>
+      <c r="M52" s="28"/>
+      <c r="N52" s="28"/>
+      <c r="O52" s="24"/>
+      <c r="P52" s="24"/>
       <c r="Q52" s="4"/>
-      <c r="R52" s="52"/>
+      <c r="R52" s="29"/>
       <c r="S52" s="4"/>
-      <c r="T52" s="53"/>
+      <c r="T52" s="30"/>
       <c r="U52" s="4"/>
     </row>
     <row r="53" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="79"/>
-      <c r="B53" s="46"/>
-      <c r="C53" s="80"/>
-      <c r="D53" s="81"/>
-      <c r="E53" s="46"/>
-      <c r="F53" s="47"/>
-      <c r="G53" s="82"/>
-      <c r="H53" s="47"/>
-      <c r="I53" s="48"/>
+      <c r="A53" s="55"/>
+      <c r="B53" s="23"/>
+      <c r="C53" s="56"/>
+      <c r="D53" s="57"/>
+      <c r="E53" s="23"/>
+      <c r="F53" s="24"/>
+      <c r="G53" s="58"/>
+      <c r="H53" s="24"/>
+      <c r="I53" s="25"/>
       <c r="J53" s="8"/>
-      <c r="K53" s="49"/>
-      <c r="L53" s="50"/>
-      <c r="M53" s="51"/>
-      <c r="N53" s="51"/>
-      <c r="O53" s="47"/>
-      <c r="P53" s="47"/>
+      <c r="K53" s="26"/>
+      <c r="L53" s="27"/>
+      <c r="M53" s="28"/>
+      <c r="N53" s="28"/>
+      <c r="O53" s="24"/>
+      <c r="P53" s="24"/>
       <c r="Q53" s="4"/>
-      <c r="R53" s="52"/>
+      <c r="R53" s="29"/>
       <c r="S53" s="4"/>
-      <c r="T53" s="53"/>
+      <c r="T53" s="30"/>
       <c r="U53" s="4"/>
     </row>
     <row r="54" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="79"/>
-      <c r="B54" s="46"/>
-      <c r="C54" s="80"/>
-      <c r="D54" s="81"/>
-      <c r="E54" s="46"/>
-      <c r="F54" s="47"/>
-      <c r="G54" s="82"/>
-      <c r="H54" s="47"/>
-      <c r="I54" s="48"/>
+      <c r="A54" s="55"/>
+      <c r="B54" s="23"/>
+      <c r="C54" s="56"/>
+      <c r="D54" s="57"/>
+      <c r="E54" s="23"/>
+      <c r="F54" s="24"/>
+      <c r="G54" s="58"/>
+      <c r="H54" s="24"/>
+      <c r="I54" s="25"/>
       <c r="J54" s="8"/>
-      <c r="K54" s="49"/>
-      <c r="L54" s="50"/>
-      <c r="M54" s="51"/>
-      <c r="N54" s="51"/>
-      <c r="O54" s="47"/>
-      <c r="P54" s="47"/>
+      <c r="K54" s="26"/>
+      <c r="L54" s="27"/>
+      <c r="M54" s="28"/>
+      <c r="N54" s="28"/>
+      <c r="O54" s="24"/>
+      <c r="P54" s="24"/>
       <c r="Q54" s="4"/>
-      <c r="R54" s="52"/>
+      <c r="R54" s="29"/>
       <c r="S54" s="4"/>
-      <c r="T54" s="53"/>
+      <c r="T54" s="30"/>
       <c r="U54" s="4"/>
     </row>
     <row r="55" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="79"/>
-      <c r="B55" s="46"/>
-      <c r="C55" s="80"/>
-      <c r="D55" s="81"/>
-      <c r="E55" s="46"/>
-      <c r="F55" s="47"/>
-      <c r="G55" s="82"/>
-      <c r="H55" s="47"/>
-      <c r="I55" s="48"/>
+      <c r="A55" s="55"/>
+      <c r="B55" s="23"/>
+      <c r="C55" s="56"/>
+      <c r="D55" s="57"/>
+      <c r="E55" s="23"/>
+      <c r="F55" s="24"/>
+      <c r="G55" s="58"/>
+      <c r="H55" s="24"/>
+      <c r="I55" s="25"/>
       <c r="J55" s="8"/>
-      <c r="K55" s="49"/>
-      <c r="L55" s="50"/>
-      <c r="M55" s="51"/>
-      <c r="N55" s="51"/>
-      <c r="O55" s="47"/>
-      <c r="P55" s="47"/>
+      <c r="K55" s="26"/>
+      <c r="L55" s="27"/>
+      <c r="M55" s="28"/>
+      <c r="N55" s="28"/>
+      <c r="O55" s="24"/>
+      <c r="P55" s="24"/>
       <c r="Q55" s="4"/>
-      <c r="R55" s="52"/>
+      <c r="R55" s="29"/>
       <c r="S55" s="4"/>
-      <c r="T55" s="53"/>
+      <c r="T55" s="30"/>
       <c r="U55" s="4"/>
     </row>
     <row r="56" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="79"/>
-      <c r="B56" s="46"/>
-      <c r="C56" s="80"/>
-      <c r="D56" s="81"/>
-      <c r="E56" s="46"/>
-      <c r="F56" s="47"/>
-      <c r="G56" s="82"/>
-      <c r="H56" s="47"/>
-      <c r="I56" s="48"/>
+      <c r="A56" s="55"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="56"/>
+      <c r="D56" s="57"/>
+      <c r="E56" s="23"/>
+      <c r="F56" s="24"/>
+      <c r="G56" s="58"/>
+      <c r="H56" s="24"/>
+      <c r="I56" s="25"/>
       <c r="J56" s="8"/>
-      <c r="K56" s="49"/>
-      <c r="L56" s="50"/>
-      <c r="M56" s="51"/>
-      <c r="N56" s="51"/>
-      <c r="O56" s="47"/>
-      <c r="P56" s="47"/>
+      <c r="K56" s="26"/>
+      <c r="L56" s="27"/>
+      <c r="M56" s="28"/>
+      <c r="N56" s="28"/>
+      <c r="O56" s="24"/>
+      <c r="P56" s="24"/>
       <c r="Q56" s="4"/>
-      <c r="R56" s="52"/>
+      <c r="R56" s="29"/>
       <c r="S56" s="4"/>
-      <c r="T56" s="53"/>
+      <c r="T56" s="30"/>
       <c r="U56" s="4"/>
     </row>
     <row r="57" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="79"/>
-      <c r="B57" s="46"/>
-      <c r="C57" s="80"/>
-      <c r="D57" s="81"/>
-      <c r="E57" s="46"/>
-      <c r="F57" s="47"/>
-      <c r="G57" s="82"/>
-      <c r="H57" s="47"/>
-      <c r="I57" s="48"/>
+      <c r="A57" s="55"/>
+      <c r="B57" s="23"/>
+      <c r="C57" s="56"/>
+      <c r="D57" s="57"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="24"/>
+      <c r="G57" s="58"/>
+      <c r="H57" s="24"/>
+      <c r="I57" s="25"/>
       <c r="J57" s="8"/>
-      <c r="K57" s="49"/>
-      <c r="L57" s="50"/>
-      <c r="M57" s="51"/>
-      <c r="N57" s="51"/>
-      <c r="O57" s="47"/>
-      <c r="P57" s="47"/>
+      <c r="K57" s="26"/>
+      <c r="L57" s="27"/>
+      <c r="M57" s="28"/>
+      <c r="N57" s="28"/>
+      <c r="O57" s="24"/>
+      <c r="P57" s="24"/>
       <c r="Q57" s="4"/>
-      <c r="R57" s="52"/>
+      <c r="R57" s="29"/>
       <c r="S57" s="4"/>
-      <c r="T57" s="53"/>
+      <c r="T57" s="30"/>
       <c r="U57" s="4"/>
     </row>
     <row r="58" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="79"/>
-      <c r="B58" s="46"/>
-      <c r="C58" s="80"/>
-      <c r="D58" s="81"/>
-      <c r="E58" s="46"/>
-      <c r="F58" s="47"/>
-      <c r="G58" s="82"/>
-      <c r="H58" s="47"/>
-      <c r="I58" s="48"/>
+      <c r="A58" s="55"/>
+      <c r="B58" s="23"/>
+      <c r="C58" s="56"/>
+      <c r="D58" s="57"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="58"/>
+      <c r="H58" s="24"/>
+      <c r="I58" s="25"/>
       <c r="J58" s="8"/>
-      <c r="K58" s="49"/>
-      <c r="L58" s="50"/>
-      <c r="M58" s="51"/>
-      <c r="N58" s="51"/>
-      <c r="O58" s="47"/>
-      <c r="P58" s="47"/>
+      <c r="K58" s="26"/>
+      <c r="L58" s="27"/>
+      <c r="M58" s="28"/>
+      <c r="N58" s="28"/>
+      <c r="O58" s="24"/>
+      <c r="P58" s="24"/>
       <c r="Q58" s="4"/>
-      <c r="R58" s="52"/>
+      <c r="R58" s="29"/>
       <c r="S58" s="4"/>
-      <c r="T58" s="53"/>
+      <c r="T58" s="30"/>
       <c r="U58" s="4"/>
     </row>
     <row r="59" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="79"/>
-      <c r="B59" s="46"/>
-      <c r="C59" s="80"/>
-      <c r="D59" s="81"/>
-      <c r="E59" s="46"/>
-      <c r="F59" s="47"/>
-      <c r="G59" s="82"/>
-      <c r="H59" s="47"/>
-      <c r="I59" s="48"/>
+      <c r="A59" s="55"/>
+      <c r="B59" s="23"/>
+      <c r="C59" s="56"/>
+      <c r="D59" s="57"/>
+      <c r="E59" s="23"/>
+      <c r="F59" s="24"/>
+      <c r="G59" s="58"/>
+      <c r="H59" s="24"/>
+      <c r="I59" s="25"/>
       <c r="J59" s="8"/>
-      <c r="K59" s="49"/>
-      <c r="L59" s="50"/>
-      <c r="M59" s="51"/>
-      <c r="N59" s="51"/>
-      <c r="O59" s="47"/>
-      <c r="P59" s="47"/>
+      <c r="K59" s="26"/>
+      <c r="L59" s="27"/>
+      <c r="M59" s="28"/>
+      <c r="N59" s="28"/>
+      <c r="O59" s="24"/>
+      <c r="P59" s="24"/>
       <c r="Q59" s="4"/>
-      <c r="R59" s="52"/>
+      <c r="R59" s="29"/>
       <c r="S59" s="4"/>
-      <c r="T59" s="53"/>
+      <c r="T59" s="30"/>
       <c r="U59" s="4"/>
     </row>
     <row r="60" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="79"/>
-      <c r="B60" s="46"/>
-      <c r="C60" s="80"/>
-      <c r="D60" s="81"/>
-      <c r="E60" s="46"/>
-      <c r="F60" s="47"/>
-      <c r="G60" s="82"/>
-      <c r="H60" s="47"/>
-      <c r="I60" s="48"/>
+      <c r="A60" s="55"/>
+      <c r="B60" s="23"/>
+      <c r="C60" s="56"/>
+      <c r="D60" s="57"/>
+      <c r="E60" s="23"/>
+      <c r="F60" s="24"/>
+      <c r="G60" s="58"/>
+      <c r="H60" s="24"/>
+      <c r="I60" s="25"/>
       <c r="J60" s="8"/>
-      <c r="K60" s="49"/>
-      <c r="L60" s="50"/>
-      <c r="M60" s="51"/>
-      <c r="N60" s="51"/>
-      <c r="O60" s="47"/>
-      <c r="P60" s="47"/>
+      <c r="K60" s="26"/>
+      <c r="L60" s="27"/>
+      <c r="M60" s="28"/>
+      <c r="N60" s="28"/>
+      <c r="O60" s="24"/>
+      <c r="P60" s="24"/>
       <c r="Q60" s="4"/>
-      <c r="R60" s="52"/>
+      <c r="R60" s="29"/>
       <c r="S60" s="4"/>
-      <c r="T60" s="53"/>
+      <c r="T60" s="30"/>
       <c r="U60" s="4"/>
     </row>
     <row r="61" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="79"/>
-      <c r="B61" s="46"/>
-      <c r="C61" s="80"/>
-      <c r="D61" s="81"/>
-      <c r="E61" s="46"/>
-      <c r="F61" s="47"/>
-      <c r="G61" s="82"/>
-      <c r="H61" s="47"/>
-      <c r="I61" s="48"/>
+      <c r="A61" s="55"/>
+      <c r="B61" s="23"/>
+      <c r="C61" s="56"/>
+      <c r="D61" s="57"/>
+      <c r="E61" s="23"/>
+      <c r="F61" s="24"/>
+      <c r="G61" s="58"/>
+      <c r="H61" s="24"/>
+      <c r="I61" s="25"/>
       <c r="J61" s="8"/>
-      <c r="K61" s="49"/>
-      <c r="L61" s="50"/>
-      <c r="M61" s="51"/>
-      <c r="N61" s="51"/>
-      <c r="O61" s="47"/>
-      <c r="P61" s="47"/>
+      <c r="K61" s="26"/>
+      <c r="L61" s="27"/>
+      <c r="M61" s="28"/>
+      <c r="N61" s="28"/>
+      <c r="O61" s="24"/>
+      <c r="P61" s="24"/>
       <c r="Q61" s="4"/>
-      <c r="R61" s="52"/>
+      <c r="R61" s="29"/>
       <c r="S61" s="4"/>
-      <c r="T61" s="53"/>
+      <c r="T61" s="30"/>
       <c r="U61" s="4"/>
     </row>
     <row r="62" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="79"/>
-      <c r="B62" s="46"/>
-      <c r="C62" s="80"/>
-      <c r="D62" s="81"/>
-      <c r="E62" s="46"/>
-      <c r="F62" s="47"/>
-      <c r="G62" s="82"/>
-      <c r="H62" s="47"/>
-      <c r="I62" s="48"/>
+      <c r="A62" s="55"/>
+      <c r="B62" s="23"/>
+      <c r="C62" s="56"/>
+      <c r="D62" s="57"/>
+      <c r="E62" s="23"/>
+      <c r="F62" s="24"/>
+      <c r="G62" s="58"/>
+      <c r="H62" s="24"/>
+      <c r="I62" s="25"/>
       <c r="J62" s="8"/>
-      <c r="K62" s="49"/>
-      <c r="L62" s="50"/>
-      <c r="M62" s="51"/>
-      <c r="N62" s="51"/>
-      <c r="O62" s="47"/>
-      <c r="P62" s="47"/>
+      <c r="K62" s="26"/>
+      <c r="L62" s="27"/>
+      <c r="M62" s="28"/>
+      <c r="N62" s="28"/>
+      <c r="O62" s="24"/>
+      <c r="P62" s="24"/>
       <c r="Q62" s="4"/>
-      <c r="R62" s="52"/>
+      <c r="R62" s="29"/>
       <c r="S62" s="4"/>
-      <c r="T62" s="53"/>
+      <c r="T62" s="30"/>
       <c r="U62" s="4"/>
     </row>
     <row r="63" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="79"/>
-      <c r="B63" s="46"/>
-      <c r="C63" s="80"/>
-      <c r="D63" s="81"/>
-      <c r="E63" s="46"/>
-      <c r="F63" s="47"/>
-      <c r="G63" s="82"/>
-      <c r="H63" s="47"/>
-      <c r="I63" s="48"/>
+      <c r="A63" s="55"/>
+      <c r="B63" s="23"/>
+      <c r="C63" s="56"/>
+      <c r="D63" s="57"/>
+      <c r="E63" s="23"/>
+      <c r="F63" s="24"/>
+      <c r="G63" s="58"/>
+      <c r="H63" s="24"/>
+      <c r="I63" s="25"/>
       <c r="J63" s="8"/>
-      <c r="K63" s="49"/>
-      <c r="L63" s="50"/>
-      <c r="M63" s="51"/>
-      <c r="N63" s="51"/>
-      <c r="O63" s="47"/>
-      <c r="P63" s="47"/>
+      <c r="K63" s="26"/>
+      <c r="L63" s="27"/>
+      <c r="M63" s="28"/>
+      <c r="N63" s="28"/>
+      <c r="O63" s="24"/>
+      <c r="P63" s="24"/>
       <c r="Q63" s="4"/>
-      <c r="R63" s="52"/>
+      <c r="R63" s="29"/>
       <c r="S63" s="4"/>
-      <c r="T63" s="53"/>
+      <c r="T63" s="30"/>
       <c r="U63" s="4"/>
     </row>
     <row r="64" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="79"/>
-      <c r="B64" s="46"/>
-      <c r="C64" s="80"/>
-      <c r="D64" s="81"/>
-      <c r="E64" s="46"/>
-      <c r="F64" s="47"/>
-      <c r="G64" s="82"/>
-      <c r="H64" s="47"/>
-      <c r="I64" s="48"/>
+      <c r="A64" s="55"/>
+      <c r="B64" s="23"/>
+      <c r="C64" s="56"/>
+      <c r="D64" s="57"/>
+      <c r="E64" s="23"/>
+      <c r="F64" s="24"/>
+      <c r="G64" s="58"/>
+      <c r="H64" s="24"/>
+      <c r="I64" s="25"/>
       <c r="J64" s="8"/>
-      <c r="K64" s="49"/>
-      <c r="L64" s="50"/>
-      <c r="M64" s="51"/>
-      <c r="N64" s="51"/>
-      <c r="O64" s="47"/>
-      <c r="P64" s="47"/>
+      <c r="K64" s="26"/>
+      <c r="L64" s="27"/>
+      <c r="M64" s="28"/>
+      <c r="N64" s="28"/>
+      <c r="O64" s="24"/>
+      <c r="P64" s="24"/>
       <c r="Q64" s="4"/>
-      <c r="R64" s="52"/>
+      <c r="R64" s="29"/>
       <c r="S64" s="4"/>
-      <c r="T64" s="53"/>
+      <c r="T64" s="30"/>
       <c r="U64" s="4"/>
     </row>
     <row r="65" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="79"/>
-      <c r="B65" s="46"/>
-      <c r="C65" s="80"/>
-      <c r="D65" s="81"/>
-      <c r="E65" s="46"/>
-      <c r="F65" s="47"/>
-      <c r="G65" s="82"/>
-      <c r="H65" s="47"/>
-      <c r="I65" s="48"/>
-      <c r="J65" s="83"/>
-      <c r="K65" s="49"/>
-      <c r="L65" s="50"/>
-      <c r="M65" s="51"/>
-      <c r="N65" s="51"/>
-      <c r="O65" s="47"/>
-      <c r="P65" s="47"/>
+      <c r="A65" s="55"/>
+      <c r="B65" s="23"/>
+      <c r="C65" s="56"/>
+      <c r="D65" s="57"/>
+      <c r="E65" s="23"/>
+      <c r="F65" s="24"/>
+      <c r="G65" s="58"/>
+      <c r="H65" s="24"/>
+      <c r="I65" s="25"/>
+      <c r="J65" s="59"/>
+      <c r="K65" s="26"/>
+      <c r="L65" s="27"/>
+      <c r="M65" s="28"/>
+      <c r="N65" s="28"/>
+      <c r="O65" s="24"/>
+      <c r="P65" s="24"/>
       <c r="Q65" s="4"/>
-      <c r="R65" s="52"/>
+      <c r="R65" s="29"/>
       <c r="S65" s="4"/>
-      <c r="T65" s="53"/>
+      <c r="T65" s="30"/>
       <c r="U65" s="4"/>
     </row>
     <row r="66" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="79"/>
-      <c r="B66" s="46"/>
-      <c r="C66" s="80"/>
-      <c r="D66" s="81"/>
-      <c r="E66" s="46"/>
-      <c r="F66" s="47"/>
-      <c r="G66" s="82"/>
-      <c r="H66" s="47"/>
-      <c r="I66" s="48"/>
-      <c r="J66" s="83"/>
-      <c r="K66" s="49"/>
-      <c r="L66" s="50"/>
-      <c r="M66" s="51"/>
-      <c r="N66" s="51"/>
-      <c r="O66" s="47"/>
-      <c r="P66" s="47"/>
+      <c r="A66" s="55"/>
+      <c r="B66" s="23"/>
+      <c r="C66" s="56"/>
+      <c r="D66" s="57"/>
+      <c r="E66" s="23"/>
+      <c r="F66" s="24"/>
+      <c r="G66" s="58"/>
+      <c r="H66" s="24"/>
+      <c r="I66" s="25"/>
+      <c r="J66" s="59"/>
+      <c r="K66" s="26"/>
+      <c r="L66" s="27"/>
+      <c r="M66" s="28"/>
+      <c r="N66" s="28"/>
+      <c r="O66" s="24"/>
+      <c r="P66" s="24"/>
       <c r="Q66" s="4"/>
-      <c r="R66" s="52"/>
+      <c r="R66" s="29"/>
       <c r="S66" s="4"/>
-      <c r="T66" s="53"/>
+      <c r="T66" s="30"/>
       <c r="U66" s="4"/>
     </row>
     <row r="67" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="79"/>
-      <c r="B67" s="46"/>
-      <c r="C67" s="80"/>
-      <c r="D67" s="81"/>
-      <c r="E67" s="46"/>
-      <c r="F67" s="47"/>
-      <c r="G67" s="82"/>
-      <c r="H67" s="47"/>
-      <c r="I67" s="48"/>
-      <c r="J67" s="83"/>
-      <c r="K67" s="49"/>
-      <c r="L67" s="50"/>
-      <c r="M67" s="51"/>
-      <c r="N67" s="51"/>
-      <c r="O67" s="47"/>
-      <c r="P67" s="47"/>
+      <c r="A67" s="55"/>
+      <c r="B67" s="23"/>
+      <c r="C67" s="56"/>
+      <c r="D67" s="57"/>
+      <c r="E67" s="23"/>
+      <c r="F67" s="24"/>
+      <c r="G67" s="58"/>
+      <c r="H67" s="24"/>
+      <c r="I67" s="25"/>
+      <c r="J67" s="59"/>
+      <c r="K67" s="26"/>
+      <c r="L67" s="27"/>
+      <c r="M67" s="28"/>
+      <c r="N67" s="28"/>
+      <c r="O67" s="24"/>
+      <c r="P67" s="24"/>
       <c r="Q67" s="4"/>
-      <c r="R67" s="52"/>
+      <c r="R67" s="29"/>
       <c r="S67" s="4"/>
-      <c r="T67" s="53"/>
+      <c r="T67" s="30"/>
       <c r="U67" s="4"/>
     </row>
     <row r="68" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="79"/>
-      <c r="B68" s="46"/>
-      <c r="C68" s="80"/>
-      <c r="D68" s="81"/>
-      <c r="E68" s="46"/>
-      <c r="F68" s="47"/>
-      <c r="G68" s="82"/>
-      <c r="H68" s="47"/>
-      <c r="I68" s="48"/>
-      <c r="J68" s="83"/>
-      <c r="K68" s="49"/>
-      <c r="L68" s="50"/>
-      <c r="M68" s="51"/>
-      <c r="N68" s="51"/>
-      <c r="O68" s="47"/>
-      <c r="P68" s="47"/>
+      <c r="A68" s="55"/>
+      <c r="B68" s="23"/>
+      <c r="C68" s="56"/>
+      <c r="D68" s="57"/>
+      <c r="E68" s="23"/>
+      <c r="F68" s="24"/>
+      <c r="G68" s="58"/>
+      <c r="H68" s="24"/>
+      <c r="I68" s="25"/>
+      <c r="J68" s="59"/>
+      <c r="K68" s="26"/>
+      <c r="L68" s="27"/>
+      <c r="M68" s="28"/>
+      <c r="N68" s="28"/>
+      <c r="O68" s="24"/>
+      <c r="P68" s="24"/>
       <c r="Q68" s="4"/>
-      <c r="R68" s="52"/>
+      <c r="R68" s="29"/>
       <c r="S68" s="4"/>
-      <c r="T68" s="53"/>
+      <c r="T68" s="30"/>
       <c r="U68" s="4"/>
     </row>
     <row r="69" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="79"/>
-      <c r="B69" s="46"/>
-      <c r="C69" s="80"/>
-      <c r="D69" s="81"/>
-      <c r="E69" s="46"/>
-      <c r="F69" s="47"/>
-      <c r="G69" s="82"/>
-      <c r="H69" s="47"/>
-      <c r="I69" s="48"/>
-      <c r="J69" s="83"/>
-      <c r="K69" s="49"/>
-      <c r="L69" s="50"/>
-      <c r="M69" s="51"/>
-      <c r="N69" s="51"/>
-      <c r="O69" s="47"/>
-      <c r="P69" s="47"/>
+      <c r="A69" s="55"/>
+      <c r="B69" s="23"/>
+      <c r="C69" s="56"/>
+      <c r="D69" s="57"/>
+      <c r="E69" s="23"/>
+      <c r="F69" s="24"/>
+      <c r="G69" s="58"/>
+      <c r="H69" s="24"/>
+      <c r="I69" s="25"/>
+      <c r="J69" s="59"/>
+      <c r="K69" s="26"/>
+      <c r="L69" s="27"/>
+      <c r="M69" s="28"/>
+      <c r="N69" s="28"/>
+      <c r="O69" s="24"/>
+      <c r="P69" s="24"/>
       <c r="Q69" s="4"/>
-      <c r="R69" s="52"/>
+      <c r="R69" s="29"/>
       <c r="S69" s="4"/>
-      <c r="T69" s="53"/>
+      <c r="T69" s="30"/>
       <c r="U69" s="4"/>
     </row>
     <row r="70" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="79"/>
-      <c r="B70" s="46"/>
-      <c r="C70" s="80"/>
-      <c r="D70" s="81"/>
-      <c r="E70" s="46"/>
-      <c r="F70" s="47"/>
-      <c r="G70" s="82"/>
-      <c r="H70" s="47"/>
-      <c r="I70" s="48"/>
-      <c r="J70" s="83"/>
-      <c r="K70" s="49"/>
-      <c r="L70" s="50"/>
-      <c r="M70" s="51"/>
-      <c r="N70" s="51"/>
-      <c r="O70" s="47"/>
-      <c r="P70" s="47"/>
+      <c r="A70" s="55"/>
+      <c r="B70" s="23"/>
+      <c r="C70" s="56"/>
+      <c r="D70" s="57"/>
+      <c r="E70" s="23"/>
+      <c r="F70" s="24"/>
+      <c r="G70" s="58"/>
+      <c r="H70" s="24"/>
+      <c r="I70" s="25"/>
+      <c r="J70" s="59"/>
+      <c r="K70" s="26"/>
+      <c r="L70" s="27"/>
+      <c r="M70" s="28"/>
+      <c r="N70" s="28"/>
+      <c r="O70" s="24"/>
+      <c r="P70" s="24"/>
       <c r="Q70" s="4"/>
-      <c r="R70" s="52"/>
+      <c r="R70" s="29"/>
       <c r="S70" s="4"/>
-      <c r="T70" s="53"/>
+      <c r="T70" s="30"/>
       <c r="U70" s="4"/>
     </row>
     <row r="71" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="79"/>
-      <c r="B71" s="46"/>
-      <c r="C71" s="80"/>
-      <c r="D71" s="81"/>
-      <c r="E71" s="46"/>
-      <c r="F71" s="47"/>
-      <c r="G71" s="82"/>
-      <c r="H71" s="47"/>
-      <c r="I71" s="48"/>
-      <c r="J71" s="83"/>
-      <c r="K71" s="49"/>
-      <c r="L71" s="50"/>
-      <c r="M71" s="51"/>
-      <c r="N71" s="51"/>
-      <c r="O71" s="47"/>
-      <c r="P71" s="47"/>
+      <c r="A71" s="55"/>
+      <c r="B71" s="23"/>
+      <c r="C71" s="56"/>
+      <c r="D71" s="57"/>
+      <c r="E71" s="23"/>
+      <c r="F71" s="24"/>
+      <c r="G71" s="58"/>
+      <c r="H71" s="24"/>
+      <c r="I71" s="25"/>
+      <c r="J71" s="59"/>
+      <c r="K71" s="26"/>
+      <c r="L71" s="27"/>
+      <c r="M71" s="28"/>
+      <c r="N71" s="28"/>
+      <c r="O71" s="24"/>
+      <c r="P71" s="24"/>
       <c r="Q71" s="4"/>
-      <c r="R71" s="52"/>
+      <c r="R71" s="29"/>
       <c r="S71" s="4"/>
-      <c r="T71" s="53"/>
+      <c r="T71" s="30"/>
       <c r="U71" s="4"/>
     </row>
     <row r="73" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
@@ -3768,187 +3770,187 @@
     <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="85" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="86" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="45" t="s">
+      <c r="A86" s="22" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="45" t="s">
+      <c r="A87" s="22" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="45" t="s">
+      <c r="A88" s="22" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="45" t="s">
+      <c r="A89" s="22" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="45" t="s">
+      <c r="A90" s="22" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="45" t="s">
+      <c r="A91" s="22" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="92" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="45" t="s">
+      <c r="A92" s="22" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="93" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="45" t="s">
+      <c r="A93" s="22" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="94" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="45" t="s">
+      <c r="A94" s="22" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="95" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="45" t="s">
+      <c r="A95" s="22" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="96" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="45" t="s">
+      <c r="A96" s="22" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="45" t="s">
+      <c r="A97" s="22" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="45" t="s">
+      <c r="A98" s="22" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="45" t="s">
+      <c r="A99" s="22" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="45" t="s">
+      <c r="A100" s="22" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="45" t="s">
+      <c r="A101" s="22" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="45" t="s">
+      <c r="A102" s="22" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="45" t="s">
+      <c r="A103" s="22" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="45" t="s">
+      <c r="A104" s="22" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="45" t="s">
+      <c r="A105" s="22" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="45" t="s">
+      <c r="A106" s="22" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="45" t="s">
+      <c r="A107" s="22" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="45" t="s">
+      <c r="A108" s="22" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="45" t="s">
+      <c r="A109" s="22" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="45" t="s">
+      <c r="A110" s="22" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="45" t="s">
+      <c r="A111" s="22" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="45" t="s">
+      <c r="A112" s="22" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="45" t="s">
+      <c r="A113" s="22" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="45" t="s">
+      <c r="A114" s="22" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="45" t="s">
+      <c r="A115" s="22" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="45" t="s">
+      <c r="A116" s="22" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="45" t="s">
+      <c r="A117" s="22" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="45" t="s">
+      <c r="A118" s="22" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="45" t="s">
+      <c r="A119" s="22" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="45" t="s">
+      <c r="A120" s="22" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="45" t="s">
+      <c r="A121" s="22" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="45" t="s">
+      <c r="A122" s="22" t="s">
         <v>115</v>
       </c>
     </row>
@@ -4120,6 +4122,12 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4134,12 +4142,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Escaletas y ajustes de recursos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion01/Escaleta_CN_11_01_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion01/Escaleta_CN_11_01_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\CienciasNaturales\fuentes\contenidos\grado11\guion01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Documents\Aula Planeta Colombia\Repositorios\CienciasNaturales\fuentes\contenidos\grado11\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,12 +18,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$2</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="204">
   <si>
     <t>Asignatura</t>
   </si>
@@ -641,7 +641,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -849,7 +849,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -946,12 +946,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1027,18 +1021,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1076,24 +1088,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1402,128 +1396,128 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W6" sqref="W6"/>
+      <selection pane="bottomLeft" activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.53125" style="22" customWidth="1"/>
+    <col min="2" max="2" width="14.3984375" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.1328125" style="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" style="60" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="75.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" style="60" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" style="60" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="112.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.28515625" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.59765625" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" style="58" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="75.265625" style="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.86328125" style="58" customWidth="1"/>
+    <col min="9" max="9" width="4.1328125" style="58" customWidth="1"/>
+    <col min="10" max="10" width="24.1328125" style="22" customWidth="1"/>
+    <col min="11" max="11" width="4.59765625" style="22" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" style="22" customWidth="1"/>
+    <col min="13" max="13" width="5.265625" style="22" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9" style="22" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="153.7109375" style="60" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.42578125" style="60" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.140625" style="60" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="44.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.85546875" style="22"/>
+    <col min="15" max="15" width="24.796875" style="58" customWidth="1"/>
+    <col min="16" max="16" width="3.265625" style="58" customWidth="1"/>
+    <col min="17" max="17" width="5.265625" style="58" customWidth="1"/>
+    <col min="18" max="18" width="4.59765625" style="22" customWidth="1"/>
+    <col min="19" max="19" width="11.796875" style="22" customWidth="1"/>
+    <col min="20" max="20" width="34.46484375" style="22" customWidth="1"/>
+    <col min="21" max="21" width="14.59765625" style="22" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.86328125" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="9" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
+    <row r="1" spans="1:21" s="9" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="D1" s="71" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="65" t="s">
+      <c r="E1" s="69" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="61" t="s">
+      <c r="F1" s="67" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="69" t="s">
+      <c r="G1" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="61" t="s">
+      <c r="H1" s="67" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="61" t="s">
+      <c r="I1" s="67" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="73" t="s">
+      <c r="J1" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="71" t="s">
+      <c r="K1" s="75" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="69" t="s">
+      <c r="L1" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="75" t="s">
+      <c r="M1" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="75"/>
-      <c r="O1" s="63" t="s">
+      <c r="N1" s="79"/>
+      <c r="O1" s="59" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="63" t="s">
+      <c r="P1" s="59" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="78" t="s">
+      <c r="Q1" s="61" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="82" t="s">
+      <c r="R1" s="65" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="78" t="s">
+      <c r="S1" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="80" t="s">
+      <c r="T1" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="78" t="s">
+      <c r="U1" s="61" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="9" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="68"/>
-      <c r="B2" s="66"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="70"/>
+    <row r="2" spans="1:21" s="9" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="72"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="74"/>
       <c r="M2" s="10" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="83"/>
-      <c r="S2" s="79"/>
-      <c r="T2" s="81"/>
-      <c r="U2" s="79"/>
-    </row>
-    <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="64"/>
+      <c r="U2" s="62"/>
+    </row>
+    <row r="3" spans="1:21" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
       <c r="A3" s="11" t="s">
         <v>17</v>
       </c>
@@ -1582,7 +1576,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A4" s="11" t="s">
         <v>17</v>
       </c>
@@ -1622,7 +1616,9 @@
         <v>23</v>
       </c>
       <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
+      <c r="P4" s="19" t="s">
+        <v>19</v>
+      </c>
       <c r="Q4" s="4">
         <v>6</v>
       </c>
@@ -1639,7 +1635,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A5" s="11" t="s">
         <v>17</v>
       </c>
@@ -1679,7 +1675,9 @@
       <c r="O5" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="P5" s="24"/>
+      <c r="P5" s="19" t="s">
+        <v>19</v>
+      </c>
       <c r="Q5" s="3" t="s">
         <v>134</v>
       </c>
@@ -1696,7 +1694,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A6" s="11" t="s">
         <v>17</v>
       </c>
@@ -1736,7 +1734,9 @@
         <v>24</v>
       </c>
       <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
+      <c r="P6" s="19" t="s">
+        <v>19</v>
+      </c>
       <c r="Q6" s="3">
         <v>6</v>
       </c>
@@ -1753,7 +1753,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A7" s="11" t="s">
         <v>17</v>
       </c>
@@ -1793,7 +1793,9 @@
         <v>33</v>
       </c>
       <c r="O7" s="24"/>
-      <c r="P7" s="24"/>
+      <c r="P7" s="19" t="s">
+        <v>19</v>
+      </c>
       <c r="Q7" s="3">
         <v>6</v>
       </c>
@@ -1810,64 +1812,66 @@
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="46" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" s="44" customFormat="1" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="13" t="s">
         <v>122</v>
       </c>
       <c r="D8" s="33" t="s">
         <v>158</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="F8" s="37"/>
-      <c r="G8" s="38" t="s">
+      <c r="F8" s="35"/>
+      <c r="G8" s="36" t="s">
         <v>148</v>
       </c>
-      <c r="H8" s="39">
+      <c r="H8" s="37">
         <v>6</v>
       </c>
-      <c r="I8" s="40" t="s">
+      <c r="I8" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="41" t="s">
+      <c r="J8" s="39" t="s">
         <v>192</v>
       </c>
-      <c r="K8" s="42" t="s">
+      <c r="K8" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="38" t="s">
+      <c r="L8" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="M8" s="43"/>
-      <c r="N8" s="43" t="s">
+      <c r="M8" s="41"/>
+      <c r="N8" s="41" t="s">
         <v>121</v>
       </c>
-      <c r="O8" s="37"/>
-      <c r="P8" s="37"/>
+      <c r="O8" s="35"/>
+      <c r="P8" s="19" t="s">
+        <v>19</v>
+      </c>
       <c r="Q8" s="6">
         <v>6</v>
       </c>
-      <c r="R8" s="44" t="s">
+      <c r="R8" s="42" t="s">
         <v>171</v>
       </c>
       <c r="S8" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="T8" s="45" t="s">
+      <c r="T8" s="43" t="s">
         <v>178</v>
       </c>
       <c r="U8" s="6" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
       <c r="A9" s="11" t="s">
         <v>17</v>
       </c>
@@ -1880,7 +1884,7 @@
       <c r="D9" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="E9" s="47" t="s">
+      <c r="E9" s="45" t="s">
         <v>143</v>
       </c>
       <c r="F9" s="19"/>
@@ -1905,7 +1909,9 @@
       <c r="M9" s="18"/>
       <c r="N9" s="18"/>
       <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
+      <c r="P9" s="19" t="s">
+        <v>19</v>
+      </c>
       <c r="Q9" s="3">
         <v>8</v>
       </c>
@@ -1922,7 +1928,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
@@ -1960,7 +1966,9 @@
       <c r="M10" s="28"/>
       <c r="N10" s="28"/>
       <c r="O10" s="24"/>
-      <c r="P10" s="24"/>
+      <c r="P10" s="19" t="s">
+        <v>19</v>
+      </c>
       <c r="Q10" s="4">
         <v>8</v>
       </c>
@@ -1977,7 +1985,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A11" s="11" t="s">
         <v>17</v>
       </c>
@@ -2017,7 +2025,9 @@
         <v>32</v>
       </c>
       <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
+      <c r="P11" s="19" t="s">
+        <v>19</v>
+      </c>
       <c r="Q11" s="3">
         <v>6</v>
       </c>
@@ -2034,64 +2044,66 @@
         <v>174</v>
       </c>
     </row>
-    <row r="12" spans="1:21" s="46" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" s="44" customFormat="1" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="13" t="s">
         <v>122</v>
       </c>
       <c r="D12" s="33" t="s">
         <v>159</v>
       </c>
-      <c r="E12" s="36" t="s">
+      <c r="E12" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="F12" s="48"/>
-      <c r="G12" s="38" t="s">
+      <c r="F12" s="46"/>
+      <c r="G12" s="36" t="s">
         <v>147</v>
       </c>
-      <c r="H12" s="39">
+      <c r="H12" s="37">
         <v>10</v>
       </c>
-      <c r="I12" s="39" t="s">
+      <c r="I12" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="41" t="s">
+      <c r="J12" s="39" t="s">
         <v>196</v>
       </c>
-      <c r="K12" s="49" t="s">
+      <c r="K12" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="L12" s="50" t="s">
+      <c r="L12" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="M12" s="51"/>
-      <c r="N12" s="51" t="s">
+      <c r="M12" s="49"/>
+      <c r="N12" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="O12" s="48"/>
-      <c r="P12" s="48"/>
+      <c r="O12" s="46"/>
+      <c r="P12" s="19" t="s">
+        <v>19</v>
+      </c>
       <c r="Q12" s="6">
         <v>6</v>
       </c>
-      <c r="R12" s="44" t="s">
+      <c r="R12" s="42" t="s">
         <v>171</v>
       </c>
       <c r="S12" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="T12" s="45" t="s">
+      <c r="T12" s="43" t="s">
         <v>179</v>
       </c>
       <c r="U12" s="6" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
       <c r="A13" s="11" t="s">
         <v>17</v>
       </c>
@@ -2104,7 +2116,7 @@
       <c r="D13" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="E13" s="47"/>
+      <c r="E13" s="45"/>
       <c r="F13" s="19"/>
       <c r="G13" s="16" t="s">
         <v>149</v>
@@ -2129,7 +2141,9 @@
       </c>
       <c r="N13" s="18"/>
       <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
+      <c r="P13" s="19" t="s">
+        <v>19</v>
+      </c>
       <c r="Q13" s="3">
         <v>6</v>
       </c>
@@ -2146,7 +2160,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A14" s="11" t="s">
         <v>17</v>
       </c>
@@ -2184,7 +2198,9 @@
         <v>33</v>
       </c>
       <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
+      <c r="P14" s="19" t="s">
+        <v>19</v>
+      </c>
       <c r="Q14" s="4">
         <v>6</v>
       </c>
@@ -2201,7 +2217,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A15" s="11" t="s">
         <v>17</v>
       </c>
@@ -2239,7 +2255,9 @@
         <v>41</v>
       </c>
       <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
+      <c r="P15" s="19" t="s">
+        <v>19</v>
+      </c>
       <c r="Q15" s="4">
         <v>6</v>
       </c>
@@ -2256,7 +2274,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A16" s="11" t="s">
         <v>17</v>
       </c>
@@ -2294,7 +2312,9 @@
         <v>32</v>
       </c>
       <c r="O16" s="24"/>
-      <c r="P16" s="24"/>
+      <c r="P16" s="19" t="s">
+        <v>19</v>
+      </c>
       <c r="Q16" s="3">
         <v>6</v>
       </c>
@@ -2311,64 +2331,66 @@
         <v>174</v>
       </c>
     </row>
-    <row r="17" spans="1:21" s="46" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" s="44" customFormat="1" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="C17" s="13" t="s">
         <v>122</v>
       </c>
       <c r="D17" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="E17" s="36" t="s">
+      <c r="E17" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="F17" s="48"/>
-      <c r="G17" s="38" t="s">
+      <c r="F17" s="46"/>
+      <c r="G17" s="36" t="s">
         <v>156</v>
       </c>
-      <c r="H17" s="39">
+      <c r="H17" s="37">
         <v>15</v>
       </c>
-      <c r="I17" s="39" t="s">
+      <c r="I17" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="41" t="s">
+      <c r="J17" s="39" t="s">
         <v>201</v>
       </c>
-      <c r="K17" s="49" t="s">
+      <c r="K17" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="L17" s="50" t="s">
+      <c r="L17" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="M17" s="51"/>
-      <c r="N17" s="51" t="s">
+      <c r="M17" s="49"/>
+      <c r="N17" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="O17" s="48"/>
-      <c r="P17" s="48"/>
+      <c r="O17" s="46"/>
+      <c r="P17" s="19" t="s">
+        <v>19</v>
+      </c>
       <c r="Q17" s="5">
         <v>6</v>
       </c>
-      <c r="R17" s="52" t="s">
+      <c r="R17" s="50" t="s">
         <v>171</v>
       </c>
       <c r="S17" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="T17" s="53" t="s">
+      <c r="T17" s="51" t="s">
         <v>180</v>
       </c>
       <c r="U17" s="5" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
       <c r="A18" s="11" t="s">
         <v>17</v>
       </c>
@@ -2381,7 +2403,7 @@
       <c r="D18" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="E18" s="47"/>
+      <c r="E18" s="45"/>
       <c r="F18" s="19"/>
       <c r="G18" s="16" t="s">
         <v>154</v>
@@ -2404,7 +2426,9 @@
       <c r="M18" s="18"/>
       <c r="N18" s="18"/>
       <c r="O18" s="19"/>
-      <c r="P18" s="19"/>
+      <c r="P18" s="19" t="s">
+        <v>19</v>
+      </c>
       <c r="Q18" s="3">
         <v>8</v>
       </c>
@@ -2421,62 +2445,64 @@
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="1:21" s="46" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" s="44" customFormat="1" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="13" t="s">
         <v>122</v>
       </c>
       <c r="D19" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="E19" s="54"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="38" t="s">
+      <c r="E19" s="52"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="36" t="s">
         <v>161</v>
       </c>
-      <c r="H19" s="39">
+      <c r="H19" s="37">
         <v>17</v>
       </c>
-      <c r="I19" s="39" t="s">
+      <c r="I19" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="41" t="s">
+      <c r="J19" s="39" t="s">
         <v>203</v>
       </c>
-      <c r="K19" s="49" t="s">
+      <c r="K19" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="L19" s="50" t="s">
+      <c r="L19" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="M19" s="51"/>
-      <c r="N19" s="51" t="s">
+      <c r="M19" s="49"/>
+      <c r="N19" s="49" t="s">
         <v>120</v>
       </c>
-      <c r="O19" s="48"/>
-      <c r="P19" s="48"/>
+      <c r="O19" s="46"/>
+      <c r="P19" s="19" t="s">
+        <v>19</v>
+      </c>
       <c r="Q19" s="6">
         <v>6</v>
       </c>
-      <c r="R19" s="44" t="s">
+      <c r="R19" s="42" t="s">
         <v>171</v>
       </c>
       <c r="S19" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="T19" s="45" t="s">
+      <c r="T19" s="43" t="s">
         <v>188</v>
       </c>
       <c r="U19" s="6" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
       <c r="A20" s="11" t="s">
         <v>17</v>
       </c>
@@ -2489,7 +2515,7 @@
       <c r="D20" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="E20" s="47"/>
+      <c r="E20" s="45"/>
       <c r="F20" s="19"/>
       <c r="G20" s="16" t="s">
         <v>10</v>
@@ -2512,14 +2538,16 @@
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
       <c r="O20" s="19"/>
-      <c r="P20" s="19"/>
+      <c r="P20" s="19" t="s">
+        <v>19</v>
+      </c>
       <c r="Q20" s="3"/>
       <c r="R20" s="20"/>
       <c r="S20" s="3"/>
       <c r="T20" s="21"/>
       <c r="U20" s="3"/>
     </row>
-    <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A21" s="11" t="s">
         <v>17</v>
       </c>
@@ -2557,7 +2585,9 @@
         <v>32</v>
       </c>
       <c r="O21" s="24"/>
-      <c r="P21" s="24"/>
+      <c r="P21" s="19" t="s">
+        <v>19</v>
+      </c>
       <c r="Q21" s="4">
         <v>6</v>
       </c>
@@ -2574,7 +2604,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A22" s="11" t="s">
         <v>17</v>
       </c>
@@ -2612,7 +2642,9 @@
         <v>52</v>
       </c>
       <c r="O22" s="24"/>
-      <c r="P22" s="24"/>
+      <c r="P22" s="19" t="s">
+        <v>19</v>
+      </c>
       <c r="Q22" s="4">
         <v>6</v>
       </c>
@@ -2629,7 +2661,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A23" s="11"/>
       <c r="B23" s="12"/>
       <c r="C23" s="13"/>
@@ -2652,7 +2684,7 @@
       <c r="T23" s="21"/>
       <c r="U23" s="3"/>
     </row>
-    <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A24" s="11"/>
       <c r="B24" s="12"/>
       <c r="C24" s="13"/>
@@ -2675,7 +2707,7 @@
       <c r="T24" s="21"/>
       <c r="U24" s="3"/>
     </row>
-    <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A25" s="11"/>
       <c r="B25" s="12"/>
       <c r="C25" s="13"/>
@@ -2698,7 +2730,7 @@
       <c r="T25" s="30"/>
       <c r="U25" s="4"/>
     </row>
-    <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A26" s="11"/>
       <c r="B26" s="12"/>
       <c r="C26" s="13"/>
@@ -2721,7 +2753,7 @@
       <c r="T26" s="30"/>
       <c r="U26" s="4"/>
     </row>
-    <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A27" s="11"/>
       <c r="B27" s="12"/>
       <c r="C27" s="13"/>
@@ -2744,7 +2776,7 @@
       <c r="T27" s="30"/>
       <c r="U27" s="4"/>
     </row>
-    <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A28" s="11"/>
       <c r="B28" s="12"/>
       <c r="C28" s="13"/>
@@ -2767,7 +2799,7 @@
       <c r="T28" s="30"/>
       <c r="U28" s="4"/>
     </row>
-    <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A29" s="11"/>
       <c r="B29" s="12"/>
       <c r="C29" s="13"/>
@@ -2790,7 +2822,7 @@
       <c r="T29" s="30"/>
       <c r="U29" s="4"/>
     </row>
-    <row r="30" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A30" s="11"/>
       <c r="B30" s="12"/>
       <c r="C30" s="13"/>
@@ -2813,7 +2845,7 @@
       <c r="T30" s="30"/>
       <c r="U30" s="4"/>
     </row>
-    <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A31" s="11"/>
       <c r="B31" s="12"/>
       <c r="C31" s="13"/>
@@ -2836,14 +2868,14 @@
       <c r="T31" s="30"/>
       <c r="U31" s="4"/>
     </row>
-    <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="55"/>
+    <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A32" s="53"/>
       <c r="B32" s="23"/>
-      <c r="C32" s="56"/>
-      <c r="D32" s="57"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="55"/>
       <c r="E32" s="23"/>
       <c r="F32" s="24"/>
-      <c r="G32" s="58"/>
+      <c r="G32" s="56"/>
       <c r="H32" s="24"/>
       <c r="I32" s="25"/>
       <c r="J32" s="8"/>
@@ -2859,14 +2891,14 @@
       <c r="T32" s="30"/>
       <c r="U32" s="4"/>
     </row>
-    <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="55"/>
+    <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A33" s="53"/>
       <c r="B33" s="23"/>
-      <c r="C33" s="56"/>
-      <c r="D33" s="57"/>
+      <c r="C33" s="54"/>
+      <c r="D33" s="55"/>
       <c r="E33" s="23"/>
       <c r="F33" s="24"/>
-      <c r="G33" s="58"/>
+      <c r="G33" s="56"/>
       <c r="H33" s="24"/>
       <c r="I33" s="25"/>
       <c r="J33" s="8"/>
@@ -2882,14 +2914,14 @@
       <c r="T33" s="30"/>
       <c r="U33" s="4"/>
     </row>
-    <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="55"/>
+    <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A34" s="53"/>
       <c r="B34" s="23"/>
-      <c r="C34" s="56"/>
-      <c r="D34" s="57"/>
+      <c r="C34" s="54"/>
+      <c r="D34" s="55"/>
       <c r="E34" s="23"/>
       <c r="F34" s="24"/>
-      <c r="G34" s="58"/>
+      <c r="G34" s="56"/>
       <c r="H34" s="24"/>
       <c r="I34" s="25"/>
       <c r="J34" s="8"/>
@@ -2905,14 +2937,14 @@
       <c r="T34" s="30"/>
       <c r="U34" s="4"/>
     </row>
-    <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="55"/>
+    <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A35" s="53"/>
       <c r="B35" s="23"/>
-      <c r="C35" s="56"/>
-      <c r="D35" s="57"/>
+      <c r="C35" s="54"/>
+      <c r="D35" s="55"/>
       <c r="E35" s="23"/>
       <c r="F35" s="24"/>
-      <c r="G35" s="58"/>
+      <c r="G35" s="56"/>
       <c r="H35" s="24"/>
       <c r="I35" s="25"/>
       <c r="J35" s="8"/>
@@ -2928,14 +2960,14 @@
       <c r="T35" s="30"/>
       <c r="U35" s="4"/>
     </row>
-    <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="55"/>
+    <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A36" s="53"/>
       <c r="B36" s="23"/>
-      <c r="C36" s="56"/>
-      <c r="D36" s="57"/>
+      <c r="C36" s="54"/>
+      <c r="D36" s="55"/>
       <c r="E36" s="23"/>
       <c r="F36" s="24"/>
-      <c r="G36" s="58"/>
+      <c r="G36" s="56"/>
       <c r="H36" s="24"/>
       <c r="I36" s="25"/>
       <c r="J36" s="8"/>
@@ -2951,14 +2983,14 @@
       <c r="T36" s="30"/>
       <c r="U36" s="4"/>
     </row>
-    <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="55"/>
+    <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A37" s="53"/>
       <c r="B37" s="23"/>
-      <c r="C37" s="56"/>
-      <c r="D37" s="57"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="55"/>
       <c r="E37" s="23"/>
       <c r="F37" s="24"/>
-      <c r="G37" s="58"/>
+      <c r="G37" s="56"/>
       <c r="H37" s="24"/>
       <c r="I37" s="25"/>
       <c r="J37" s="8"/>
@@ -2974,14 +3006,14 @@
       <c r="T37" s="30"/>
       <c r="U37" s="4"/>
     </row>
-    <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="55"/>
+    <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A38" s="53"/>
       <c r="B38" s="23"/>
-      <c r="C38" s="56"/>
-      <c r="D38" s="57"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="55"/>
       <c r="E38" s="23"/>
       <c r="F38" s="24"/>
-      <c r="G38" s="58"/>
+      <c r="G38" s="56"/>
       <c r="H38" s="24"/>
       <c r="I38" s="25"/>
       <c r="J38" s="8"/>
@@ -2997,14 +3029,14 @@
       <c r="T38" s="30"/>
       <c r="U38" s="4"/>
     </row>
-    <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="55"/>
+    <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A39" s="53"/>
       <c r="B39" s="23"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="57"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="55"/>
       <c r="E39" s="23"/>
       <c r="F39" s="24"/>
-      <c r="G39" s="58"/>
+      <c r="G39" s="56"/>
       <c r="H39" s="24"/>
       <c r="I39" s="25"/>
       <c r="J39" s="8"/>
@@ -3020,14 +3052,14 @@
       <c r="T39" s="30"/>
       <c r="U39" s="4"/>
     </row>
-    <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="55"/>
+    <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A40" s="53"/>
       <c r="B40" s="23"/>
-      <c r="C40" s="56"/>
-      <c r="D40" s="57"/>
+      <c r="C40" s="54"/>
+      <c r="D40" s="55"/>
       <c r="E40" s="23"/>
       <c r="F40" s="24"/>
-      <c r="G40" s="58"/>
+      <c r="G40" s="56"/>
       <c r="H40" s="24"/>
       <c r="I40" s="25"/>
       <c r="J40" s="8"/>
@@ -3043,14 +3075,14 @@
       <c r="T40" s="30"/>
       <c r="U40" s="4"/>
     </row>
-    <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="55"/>
+    <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A41" s="53"/>
       <c r="B41" s="23"/>
-      <c r="C41" s="56"/>
-      <c r="D41" s="57"/>
+      <c r="C41" s="54"/>
+      <c r="D41" s="55"/>
       <c r="E41" s="23"/>
       <c r="F41" s="24"/>
-      <c r="G41" s="58"/>
+      <c r="G41" s="56"/>
       <c r="H41" s="24"/>
       <c r="I41" s="25"/>
       <c r="J41" s="8"/>
@@ -3066,14 +3098,14 @@
       <c r="T41" s="30"/>
       <c r="U41" s="4"/>
     </row>
-    <row r="42" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="55"/>
+    <row r="42" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A42" s="53"/>
       <c r="B42" s="23"/>
-      <c r="C42" s="56"/>
-      <c r="D42" s="57"/>
+      <c r="C42" s="54"/>
+      <c r="D42" s="55"/>
       <c r="E42" s="23"/>
       <c r="F42" s="24"/>
-      <c r="G42" s="58"/>
+      <c r="G42" s="56"/>
       <c r="H42" s="24"/>
       <c r="I42" s="25"/>
       <c r="J42" s="8"/>
@@ -3089,14 +3121,14 @@
       <c r="T42" s="30"/>
       <c r="U42" s="4"/>
     </row>
-    <row r="43" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="55"/>
+    <row r="43" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A43" s="53"/>
       <c r="B43" s="23"/>
-      <c r="C43" s="56"/>
-      <c r="D43" s="57"/>
+      <c r="C43" s="54"/>
+      <c r="D43" s="55"/>
       <c r="E43" s="23"/>
       <c r="F43" s="24"/>
-      <c r="G43" s="58"/>
+      <c r="G43" s="56"/>
       <c r="H43" s="24"/>
       <c r="I43" s="25"/>
       <c r="J43" s="8"/>
@@ -3112,14 +3144,14 @@
       <c r="T43" s="30"/>
       <c r="U43" s="4"/>
     </row>
-    <row r="44" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="55"/>
+    <row r="44" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A44" s="53"/>
       <c r="B44" s="23"/>
-      <c r="C44" s="56"/>
-      <c r="D44" s="57"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="55"/>
       <c r="E44" s="23"/>
       <c r="F44" s="24"/>
-      <c r="G44" s="58"/>
+      <c r="G44" s="56"/>
       <c r="H44" s="24"/>
       <c r="I44" s="25"/>
       <c r="J44" s="8"/>
@@ -3135,14 +3167,14 @@
       <c r="T44" s="30"/>
       <c r="U44" s="4"/>
     </row>
-    <row r="45" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="55"/>
+    <row r="45" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A45" s="53"/>
       <c r="B45" s="23"/>
-      <c r="C45" s="56"/>
-      <c r="D45" s="57"/>
+      <c r="C45" s="54"/>
+      <c r="D45" s="55"/>
       <c r="E45" s="23"/>
       <c r="F45" s="24"/>
-      <c r="G45" s="58"/>
+      <c r="G45" s="56"/>
       <c r="H45" s="24"/>
       <c r="I45" s="25"/>
       <c r="J45" s="8"/>
@@ -3158,14 +3190,14 @@
       <c r="T45" s="30"/>
       <c r="U45" s="4"/>
     </row>
-    <row r="46" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="55"/>
+    <row r="46" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A46" s="53"/>
       <c r="B46" s="23"/>
-      <c r="C46" s="56"/>
-      <c r="D46" s="57"/>
+      <c r="C46" s="54"/>
+      <c r="D46" s="55"/>
       <c r="E46" s="23"/>
       <c r="F46" s="24"/>
-      <c r="G46" s="58"/>
+      <c r="G46" s="56"/>
       <c r="H46" s="24"/>
       <c r="I46" s="25"/>
       <c r="J46" s="8"/>
@@ -3181,14 +3213,14 @@
       <c r="T46" s="30"/>
       <c r="U46" s="4"/>
     </row>
-    <row r="47" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="55"/>
+    <row r="47" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A47" s="53"/>
       <c r="B47" s="23"/>
-      <c r="C47" s="56"/>
-      <c r="D47" s="57"/>
+      <c r="C47" s="54"/>
+      <c r="D47" s="55"/>
       <c r="E47" s="23"/>
       <c r="F47" s="24"/>
-      <c r="G47" s="58"/>
+      <c r="G47" s="56"/>
       <c r="H47" s="24"/>
       <c r="I47" s="25"/>
       <c r="J47" s="8"/>
@@ -3204,14 +3236,14 @@
       <c r="T47" s="30"/>
       <c r="U47" s="4"/>
     </row>
-    <row r="48" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="55"/>
+    <row r="48" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A48" s="53"/>
       <c r="B48" s="23"/>
-      <c r="C48" s="56"/>
-      <c r="D48" s="57"/>
+      <c r="C48" s="54"/>
+      <c r="D48" s="55"/>
       <c r="E48" s="23"/>
       <c r="F48" s="24"/>
-      <c r="G48" s="58"/>
+      <c r="G48" s="56"/>
       <c r="H48" s="24"/>
       <c r="I48" s="25"/>
       <c r="J48" s="8"/>
@@ -3227,14 +3259,14 @@
       <c r="T48" s="30"/>
       <c r="U48" s="4"/>
     </row>
-    <row r="49" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="55"/>
+    <row r="49" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A49" s="53"/>
       <c r="B49" s="23"/>
-      <c r="C49" s="56"/>
-      <c r="D49" s="57"/>
+      <c r="C49" s="54"/>
+      <c r="D49" s="55"/>
       <c r="E49" s="23"/>
       <c r="F49" s="24"/>
-      <c r="G49" s="58"/>
+      <c r="G49" s="56"/>
       <c r="H49" s="24"/>
       <c r="I49" s="25"/>
       <c r="J49" s="8"/>
@@ -3250,14 +3282,14 @@
       <c r="T49" s="30"/>
       <c r="U49" s="4"/>
     </row>
-    <row r="50" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="55"/>
+    <row r="50" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A50" s="53"/>
       <c r="B50" s="23"/>
-      <c r="C50" s="56"/>
-      <c r="D50" s="57"/>
+      <c r="C50" s="54"/>
+      <c r="D50" s="55"/>
       <c r="E50" s="23"/>
       <c r="F50" s="24"/>
-      <c r="G50" s="58"/>
+      <c r="G50" s="56"/>
       <c r="H50" s="24"/>
       <c r="I50" s="25"/>
       <c r="J50" s="8"/>
@@ -3273,14 +3305,14 @@
       <c r="T50" s="30"/>
       <c r="U50" s="4"/>
     </row>
-    <row r="51" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="55"/>
+    <row r="51" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A51" s="53"/>
       <c r="B51" s="23"/>
-      <c r="C51" s="56"/>
-      <c r="D51" s="57"/>
+      <c r="C51" s="54"/>
+      <c r="D51" s="55"/>
       <c r="E51" s="23"/>
       <c r="F51" s="24"/>
-      <c r="G51" s="58"/>
+      <c r="G51" s="56"/>
       <c r="H51" s="24"/>
       <c r="I51" s="25"/>
       <c r="J51" s="8"/>
@@ -3296,14 +3328,14 @@
       <c r="T51" s="30"/>
       <c r="U51" s="4"/>
     </row>
-    <row r="52" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="55"/>
+    <row r="52" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A52" s="53"/>
       <c r="B52" s="23"/>
-      <c r="C52" s="56"/>
-      <c r="D52" s="57"/>
+      <c r="C52" s="54"/>
+      <c r="D52" s="55"/>
       <c r="E52" s="23"/>
       <c r="F52" s="24"/>
-      <c r="G52" s="58"/>
+      <c r="G52" s="56"/>
       <c r="H52" s="24"/>
       <c r="I52" s="25"/>
       <c r="J52" s="8"/>
@@ -3319,14 +3351,14 @@
       <c r="T52" s="30"/>
       <c r="U52" s="4"/>
     </row>
-    <row r="53" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="55"/>
+    <row r="53" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A53" s="53"/>
       <c r="B53" s="23"/>
-      <c r="C53" s="56"/>
-      <c r="D53" s="57"/>
+      <c r="C53" s="54"/>
+      <c r="D53" s="55"/>
       <c r="E53" s="23"/>
       <c r="F53" s="24"/>
-      <c r="G53" s="58"/>
+      <c r="G53" s="56"/>
       <c r="H53" s="24"/>
       <c r="I53" s="25"/>
       <c r="J53" s="8"/>
@@ -3342,14 +3374,14 @@
       <c r="T53" s="30"/>
       <c r="U53" s="4"/>
     </row>
-    <row r="54" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="55"/>
+    <row r="54" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A54" s="53"/>
       <c r="B54" s="23"/>
-      <c r="C54" s="56"/>
-      <c r="D54" s="57"/>
+      <c r="C54" s="54"/>
+      <c r="D54" s="55"/>
       <c r="E54" s="23"/>
       <c r="F54" s="24"/>
-      <c r="G54" s="58"/>
+      <c r="G54" s="56"/>
       <c r="H54" s="24"/>
       <c r="I54" s="25"/>
       <c r="J54" s="8"/>
@@ -3365,14 +3397,14 @@
       <c r="T54" s="30"/>
       <c r="U54" s="4"/>
     </row>
-    <row r="55" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="55"/>
+    <row r="55" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A55" s="53"/>
       <c r="B55" s="23"/>
-      <c r="C55" s="56"/>
-      <c r="D55" s="57"/>
+      <c r="C55" s="54"/>
+      <c r="D55" s="55"/>
       <c r="E55" s="23"/>
       <c r="F55" s="24"/>
-      <c r="G55" s="58"/>
+      <c r="G55" s="56"/>
       <c r="H55" s="24"/>
       <c r="I55" s="25"/>
       <c r="J55" s="8"/>
@@ -3388,14 +3420,14 @@
       <c r="T55" s="30"/>
       <c r="U55" s="4"/>
     </row>
-    <row r="56" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="55"/>
+    <row r="56" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A56" s="53"/>
       <c r="B56" s="23"/>
-      <c r="C56" s="56"/>
-      <c r="D56" s="57"/>
+      <c r="C56" s="54"/>
+      <c r="D56" s="55"/>
       <c r="E56" s="23"/>
       <c r="F56" s="24"/>
-      <c r="G56" s="58"/>
+      <c r="G56" s="56"/>
       <c r="H56" s="24"/>
       <c r="I56" s="25"/>
       <c r="J56" s="8"/>
@@ -3411,14 +3443,14 @@
       <c r="T56" s="30"/>
       <c r="U56" s="4"/>
     </row>
-    <row r="57" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="55"/>
+    <row r="57" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A57" s="53"/>
       <c r="B57" s="23"/>
-      <c r="C57" s="56"/>
-      <c r="D57" s="57"/>
+      <c r="C57" s="54"/>
+      <c r="D57" s="55"/>
       <c r="E57" s="23"/>
       <c r="F57" s="24"/>
-      <c r="G57" s="58"/>
+      <c r="G57" s="56"/>
       <c r="H57" s="24"/>
       <c r="I57" s="25"/>
       <c r="J57" s="8"/>
@@ -3434,14 +3466,14 @@
       <c r="T57" s="30"/>
       <c r="U57" s="4"/>
     </row>
-    <row r="58" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="55"/>
+    <row r="58" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A58" s="53"/>
       <c r="B58" s="23"/>
-      <c r="C58" s="56"/>
-      <c r="D58" s="57"/>
+      <c r="C58" s="54"/>
+      <c r="D58" s="55"/>
       <c r="E58" s="23"/>
       <c r="F58" s="24"/>
-      <c r="G58" s="58"/>
+      <c r="G58" s="56"/>
       <c r="H58" s="24"/>
       <c r="I58" s="25"/>
       <c r="J58" s="8"/>
@@ -3457,14 +3489,14 @@
       <c r="T58" s="30"/>
       <c r="U58" s="4"/>
     </row>
-    <row r="59" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="55"/>
+    <row r="59" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A59" s="53"/>
       <c r="B59" s="23"/>
-      <c r="C59" s="56"/>
-      <c r="D59" s="57"/>
+      <c r="C59" s="54"/>
+      <c r="D59" s="55"/>
       <c r="E59" s="23"/>
       <c r="F59" s="24"/>
-      <c r="G59" s="58"/>
+      <c r="G59" s="56"/>
       <c r="H59" s="24"/>
       <c r="I59" s="25"/>
       <c r="J59" s="8"/>
@@ -3480,14 +3512,14 @@
       <c r="T59" s="30"/>
       <c r="U59" s="4"/>
     </row>
-    <row r="60" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="55"/>
+    <row r="60" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A60" s="53"/>
       <c r="B60" s="23"/>
-      <c r="C60" s="56"/>
-      <c r="D60" s="57"/>
+      <c r="C60" s="54"/>
+      <c r="D60" s="55"/>
       <c r="E60" s="23"/>
       <c r="F60" s="24"/>
-      <c r="G60" s="58"/>
+      <c r="G60" s="56"/>
       <c r="H60" s="24"/>
       <c r="I60" s="25"/>
       <c r="J60" s="8"/>
@@ -3503,14 +3535,14 @@
       <c r="T60" s="30"/>
       <c r="U60" s="4"/>
     </row>
-    <row r="61" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="55"/>
+    <row r="61" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A61" s="53"/>
       <c r="B61" s="23"/>
-      <c r="C61" s="56"/>
-      <c r="D61" s="57"/>
+      <c r="C61" s="54"/>
+      <c r="D61" s="55"/>
       <c r="E61" s="23"/>
       <c r="F61" s="24"/>
-      <c r="G61" s="58"/>
+      <c r="G61" s="56"/>
       <c r="H61" s="24"/>
       <c r="I61" s="25"/>
       <c r="J61" s="8"/>
@@ -3526,14 +3558,14 @@
       <c r="T61" s="30"/>
       <c r="U61" s="4"/>
     </row>
-    <row r="62" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="55"/>
+    <row r="62" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A62" s="53"/>
       <c r="B62" s="23"/>
-      <c r="C62" s="56"/>
-      <c r="D62" s="57"/>
+      <c r="C62" s="54"/>
+      <c r="D62" s="55"/>
       <c r="E62" s="23"/>
       <c r="F62" s="24"/>
-      <c r="G62" s="58"/>
+      <c r="G62" s="56"/>
       <c r="H62" s="24"/>
       <c r="I62" s="25"/>
       <c r="J62" s="8"/>
@@ -3549,14 +3581,14 @@
       <c r="T62" s="30"/>
       <c r="U62" s="4"/>
     </row>
-    <row r="63" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="55"/>
+    <row r="63" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A63" s="53"/>
       <c r="B63" s="23"/>
-      <c r="C63" s="56"/>
-      <c r="D63" s="57"/>
+      <c r="C63" s="54"/>
+      <c r="D63" s="55"/>
       <c r="E63" s="23"/>
       <c r="F63" s="24"/>
-      <c r="G63" s="58"/>
+      <c r="G63" s="56"/>
       <c r="H63" s="24"/>
       <c r="I63" s="25"/>
       <c r="J63" s="8"/>
@@ -3572,14 +3604,14 @@
       <c r="T63" s="30"/>
       <c r="U63" s="4"/>
     </row>
-    <row r="64" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="55"/>
+    <row r="64" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A64" s="53"/>
       <c r="B64" s="23"/>
-      <c r="C64" s="56"/>
-      <c r="D64" s="57"/>
+      <c r="C64" s="54"/>
+      <c r="D64" s="55"/>
       <c r="E64" s="23"/>
       <c r="F64" s="24"/>
-      <c r="G64" s="58"/>
+      <c r="G64" s="56"/>
       <c r="H64" s="24"/>
       <c r="I64" s="25"/>
       <c r="J64" s="8"/>
@@ -3595,17 +3627,17 @@
       <c r="T64" s="30"/>
       <c r="U64" s="4"/>
     </row>
-    <row r="65" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="55"/>
+    <row r="65" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A65" s="53"/>
       <c r="B65" s="23"/>
-      <c r="C65" s="56"/>
-      <c r="D65" s="57"/>
+      <c r="C65" s="54"/>
+      <c r="D65" s="55"/>
       <c r="E65" s="23"/>
       <c r="F65" s="24"/>
-      <c r="G65" s="58"/>
+      <c r="G65" s="56"/>
       <c r="H65" s="24"/>
       <c r="I65" s="25"/>
-      <c r="J65" s="59"/>
+      <c r="J65" s="57"/>
       <c r="K65" s="26"/>
       <c r="L65" s="27"/>
       <c r="M65" s="28"/>
@@ -3618,17 +3650,17 @@
       <c r="T65" s="30"/>
       <c r="U65" s="4"/>
     </row>
-    <row r="66" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="55"/>
+    <row r="66" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A66" s="53"/>
       <c r="B66" s="23"/>
-      <c r="C66" s="56"/>
-      <c r="D66" s="57"/>
+      <c r="C66" s="54"/>
+      <c r="D66" s="55"/>
       <c r="E66" s="23"/>
       <c r="F66" s="24"/>
-      <c r="G66" s="58"/>
+      <c r="G66" s="56"/>
       <c r="H66" s="24"/>
       <c r="I66" s="25"/>
-      <c r="J66" s="59"/>
+      <c r="J66" s="57"/>
       <c r="K66" s="26"/>
       <c r="L66" s="27"/>
       <c r="M66" s="28"/>
@@ -3641,17 +3673,17 @@
       <c r="T66" s="30"/>
       <c r="U66" s="4"/>
     </row>
-    <row r="67" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="55"/>
+    <row r="67" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A67" s="53"/>
       <c r="B67" s="23"/>
-      <c r="C67" s="56"/>
-      <c r="D67" s="57"/>
+      <c r="C67" s="54"/>
+      <c r="D67" s="55"/>
       <c r="E67" s="23"/>
       <c r="F67" s="24"/>
-      <c r="G67" s="58"/>
+      <c r="G67" s="56"/>
       <c r="H67" s="24"/>
       <c r="I67" s="25"/>
-      <c r="J67" s="59"/>
+      <c r="J67" s="57"/>
       <c r="K67" s="26"/>
       <c r="L67" s="27"/>
       <c r="M67" s="28"/>
@@ -3664,17 +3696,17 @@
       <c r="T67" s="30"/>
       <c r="U67" s="4"/>
     </row>
-    <row r="68" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="55"/>
+    <row r="68" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A68" s="53"/>
       <c r="B68" s="23"/>
-      <c r="C68" s="56"/>
-      <c r="D68" s="57"/>
+      <c r="C68" s="54"/>
+      <c r="D68" s="55"/>
       <c r="E68" s="23"/>
       <c r="F68" s="24"/>
-      <c r="G68" s="58"/>
+      <c r="G68" s="56"/>
       <c r="H68" s="24"/>
       <c r="I68" s="25"/>
-      <c r="J68" s="59"/>
+      <c r="J68" s="57"/>
       <c r="K68" s="26"/>
       <c r="L68" s="27"/>
       <c r="M68" s="28"/>
@@ -3687,17 +3719,17 @@
       <c r="T68" s="30"/>
       <c r="U68" s="4"/>
     </row>
-    <row r="69" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="55"/>
+    <row r="69" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A69" s="53"/>
       <c r="B69" s="23"/>
-      <c r="C69" s="56"/>
-      <c r="D69" s="57"/>
+      <c r="C69" s="54"/>
+      <c r="D69" s="55"/>
       <c r="E69" s="23"/>
       <c r="F69" s="24"/>
-      <c r="G69" s="58"/>
+      <c r="G69" s="56"/>
       <c r="H69" s="24"/>
       <c r="I69" s="25"/>
-      <c r="J69" s="59"/>
+      <c r="J69" s="57"/>
       <c r="K69" s="26"/>
       <c r="L69" s="27"/>
       <c r="M69" s="28"/>
@@ -3710,17 +3742,17 @@
       <c r="T69" s="30"/>
       <c r="U69" s="4"/>
     </row>
-    <row r="70" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="55"/>
+    <row r="70" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A70" s="53"/>
       <c r="B70" s="23"/>
-      <c r="C70" s="56"/>
-      <c r="D70" s="57"/>
+      <c r="C70" s="54"/>
+      <c r="D70" s="55"/>
       <c r="E70" s="23"/>
       <c r="F70" s="24"/>
-      <c r="G70" s="58"/>
+      <c r="G70" s="56"/>
       <c r="H70" s="24"/>
       <c r="I70" s="25"/>
-      <c r="J70" s="59"/>
+      <c r="J70" s="57"/>
       <c r="K70" s="26"/>
       <c r="L70" s="27"/>
       <c r="M70" s="28"/>
@@ -3733,17 +3765,17 @@
       <c r="T70" s="30"/>
       <c r="U70" s="4"/>
     </row>
-    <row r="71" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="55"/>
+    <row r="71" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A71" s="53"/>
       <c r="B71" s="23"/>
-      <c r="C71" s="56"/>
-      <c r="D71" s="57"/>
+      <c r="C71" s="54"/>
+      <c r="D71" s="55"/>
       <c r="E71" s="23"/>
       <c r="F71" s="24"/>
-      <c r="G71" s="58"/>
+      <c r="G71" s="56"/>
       <c r="H71" s="24"/>
       <c r="I71" s="25"/>
-      <c r="J71" s="59"/>
+      <c r="J71" s="57"/>
       <c r="K71" s="26"/>
       <c r="L71" s="27"/>
       <c r="M71" s="28"/>
@@ -3756,378 +3788,372 @@
       <c r="T71" s="30"/>
       <c r="U71" s="4"/>
     </row>
-    <row r="73" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="76" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="81" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="82" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="83" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="85" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="86" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:21" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="74" spans="1:21" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="75" spans="1:21" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="76" spans="1:21" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="77" spans="1:21" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="78" spans="1:21" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="79" spans="1:21" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="80" spans="1:21" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="81" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="82" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="83" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="85" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="86" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A86" s="22" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A87" s="22" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A88" s="22" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A89" s="22" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A90" s="22" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A91" s="22" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="92" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A92" s="22" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="93" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A93" s="22" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="94" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A94" s="22" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="95" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A95" s="22" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="96" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A96" s="22" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A97" s="22" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A98" s="22" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A99" s="22" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A100" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A101" s="22" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A102" s="22" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A103" s="22" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A104" s="22" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A105" s="22" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A106" s="22" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A107" s="22" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A108" s="22" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A109" s="22" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A110" s="22" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A111" s="22" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A112" s="22" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A113" s="22" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A114" s="22" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A115" s="22" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A116" s="22" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A117" s="22" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A118" s="22" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A119" s="22" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A120" s="22" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A121" s="22" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A122" s="22" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="126" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="127" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="128" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="129" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="130" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="131" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="132" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="133" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="134" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="135" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="136" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="137" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="138" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="139" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="140" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="141" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="142" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="143" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="144" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="145" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="146" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="147" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="148" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="149" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="150" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="151" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="152" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="153" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="154" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="155" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="156" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="157" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="158" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="159" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="160" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="161" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="162" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="163" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="164" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="165" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="166" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="167" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="168" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="169" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="170" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="171" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="172" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="173" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="174" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="175" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="176" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="177" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="178" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="179" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="180" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="181" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="182" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="183" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="184" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="185" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="186" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="187" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="188" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="189" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="190" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="191" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="192" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="193" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="194" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="195" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="196" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="197" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="198" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="199" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="200" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="201" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="202" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="203" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="204" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="205" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="206" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="207" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="208" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="209" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="210" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="211" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="212" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="213" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="214" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="215" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="216" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="217" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="218" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="219" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="220" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="221" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="222" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="223" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="224" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="225" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="226" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="227" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="228" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="229" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="230" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="231" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="232" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="233" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="234" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="235" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="236" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="237" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="238" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="239" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="240" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="241" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="242" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="243" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="244" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="245" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="246" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="247" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="248" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="249" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="250" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="251" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="252" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="253" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="254" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="255" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="256" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="257" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="258" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="259" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="260" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="261" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="262" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="263" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="264" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="265" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="266" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="267" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="268" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="269" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="270" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="271" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="272" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="273" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="274" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="275" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="276" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="277" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="278" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="279" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="280" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="281" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="282" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="283" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="284" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="285" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="126" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="127" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="128" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="129" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="130" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="131" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="132" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="133" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="134" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="135" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="136" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="137" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="138" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="139" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="140" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="141" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="142" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="143" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="144" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="145" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="146" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="147" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="148" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="149" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="150" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="151" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="152" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="153" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="154" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="155" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="156" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="157" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="158" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="159" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="160" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="161" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="162" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="163" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="164" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="165" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="166" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="167" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="168" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="169" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="170" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="171" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="172" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="173" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="174" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="175" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="176" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="177" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="178" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="179" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="180" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="181" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="182" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="183" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="184" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="185" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="186" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="187" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="188" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="189" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="190" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="191" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="192" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="193" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="194" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="195" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="196" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="197" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="198" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="199" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="200" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="201" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="202" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="203" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="204" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="205" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="206" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="207" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="208" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="209" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="210" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="211" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="212" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="213" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="214" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="215" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="216" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="217" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="218" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="219" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="220" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="221" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="222" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="223" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="224" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="225" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="226" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="227" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="228" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="229" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="230" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="231" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="232" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="233" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="234" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="235" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="236" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="237" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="238" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="239" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="240" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="241" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="242" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="243" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="244" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="245" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="246" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="247" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="248" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="249" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="250" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="251" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="252" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="253" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="254" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="255" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="256" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="257" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="258" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="259" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="260" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="261" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="262" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="263" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="264" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="265" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="266" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="267" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="268" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="269" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="270" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="271" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="272" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="273" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="274" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="275" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="276" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="277" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="278" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="279" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="280" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="281" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="282" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="283" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="284" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="285" hidden="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <autoFilter ref="A1:U2">
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4142,6 +4168,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -4192,27 +4224,27 @@
       <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.86328125" style="1" customWidth="1"/>
     <col min="4" max="4" width="34" style="1" customWidth="1"/>
-    <col min="5" max="5" width="34.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.86328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.3984375" style="1" customWidth="1"/>
     <col min="7" max="7" width="18" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.86328125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.3984375" style="1" customWidth="1"/>
     <col min="12" max="12" width="17" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="1"/>
-    <col min="14" max="14" width="24.140625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="69.85546875" style="1" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.42578125" style="1"/>
+    <col min="13" max="13" width="11.3984375" style="1"/>
+    <col min="14" max="14" width="24.1328125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="69.86328125" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.3984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -4229,7 +4261,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -4253,7 +4285,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -4272,7 +4304,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -4291,7 +4323,7 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
@@ -4307,7 +4339,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
@@ -4324,7 +4356,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
@@ -4341,7 +4373,7 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -4356,7 +4388,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -4371,7 +4403,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -4386,7 +4418,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -4401,7 +4433,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -4416,7 +4448,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -4431,7 +4463,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -4446,7 +4478,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -4461,7 +4493,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -4476,7 +4508,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="1" t="s">
@@ -4490,7 +4522,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="1" t="s">
@@ -4504,7 +4536,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="1" t="s">
@@ -4518,7 +4550,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="1" t="s">
@@ -4532,7 +4564,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -4547,7 +4579,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -4562,7 +4594,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -4577,7 +4609,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -4592,7 +4624,7 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -4607,7 +4639,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -4622,7 +4654,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -4637,7 +4669,7 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -4652,7 +4684,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -4667,7 +4699,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -4682,7 +4714,7 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -4697,7 +4729,7 @@
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -4712,7 +4744,7 @@
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -4727,7 +4759,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -4742,7 +4774,7 @@
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -4757,7 +4789,7 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -4772,7 +4804,7 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -4787,7 +4819,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -4802,7 +4834,7 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -4817,7 +4849,7 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -4832,7 +4864,7 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -4847,7 +4879,7 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -4862,7 +4894,7 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -4877,7 +4909,7 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -4892,7 +4924,7 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -4907,7 +4939,7 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -4922,7 +4954,7 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -4937,7 +4969,7 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -4952,7 +4984,7 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -4964,7 +4996,7 @@
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
     </row>
-    <row r="50" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -4976,7 +5008,7 @@
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
     </row>
-    <row r="51" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -4989,7 +5021,7 @@
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
     </row>
-    <row r="52" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -5002,7 +5034,7 @@
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
     </row>
-    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -5015,7 +5047,7 @@
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
     </row>
-    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -5028,7 +5060,7 @@
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
     </row>
-    <row r="55" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -5041,7 +5073,7 @@
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
     </row>
-    <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -5054,7 +5086,7 @@
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
     </row>
-    <row r="57" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -5067,7 +5099,7 @@
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
     </row>
-    <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -5080,7 +5112,7 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
     </row>
-    <row r="59" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -5093,7 +5125,7 @@
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
     </row>
-    <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -5106,7 +5138,7 @@
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
     </row>
-    <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -5119,7 +5151,7 @@
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
     </row>
-    <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -5132,7 +5164,7 @@
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
     </row>
-    <row r="63" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -5145,7 +5177,7 @@
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
     </row>
-    <row r="64" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -5158,7 +5190,7 @@
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
     </row>
-    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -5171,7 +5203,7 @@
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
     </row>
-    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
@@ -5184,7 +5216,7 @@
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
     </row>
-    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
@@ -5197,7 +5229,7 @@
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
     </row>
-    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -5210,7 +5242,7 @@
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
     </row>
-    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -5223,7 +5255,7 @@
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
     </row>
-    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
@@ -5236,7 +5268,7 @@
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
     </row>
-    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -5250,7 +5282,7 @@
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
     </row>
-    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -5264,7 +5296,7 @@
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
     </row>
-    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -5278,7 +5310,7 @@
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
     </row>
-    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -5292,7 +5324,7 @@
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
     </row>
-    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -5306,7 +5338,7 @@
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
     </row>
-    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -5320,7 +5352,7 @@
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
     </row>
-    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -5334,7 +5366,7 @@
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
     </row>
-    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -5348,7 +5380,7 @@
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
     </row>
-    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -5362,7 +5394,7 @@
       <c r="K79" s="2"/>
       <c r="L79" s="2"/>
     </row>
-    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -5376,7 +5408,7 @@
       <c r="K80" s="2"/>
       <c r="L80" s="2"/>
     </row>
-    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -5390,7 +5422,7 @@
       <c r="K81" s="2"/>
       <c r="L81" s="2"/>
     </row>
-    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -5404,7 +5436,7 @@
       <c r="K82" s="2"/>
       <c r="L82" s="2"/>
     </row>
-    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -5418,7 +5450,7 @@
       <c r="K83" s="2"/>
       <c r="L83" s="2"/>
     </row>
-    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -5432,7 +5464,7 @@
       <c r="K84" s="2"/>
       <c r="L84" s="2"/>
     </row>
-    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -5446,7 +5478,7 @@
       <c r="K85" s="2"/>
       <c r="L85" s="2"/>
     </row>
-    <row r="86" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -5460,7 +5492,7 @@
       <c r="K86" s="2"/>
       <c r="L86" s="2"/>
     </row>
-    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -5474,7 +5506,7 @@
       <c r="K87" s="2"/>
       <c r="L87" s="2"/>
     </row>
-    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -5488,7 +5520,7 @@
       <c r="K88" s="2"/>
       <c r="L88" s="2"/>
     </row>
-    <row r="89" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -5502,7 +5534,7 @@
       <c r="K89" s="2"/>
       <c r="L89" s="2"/>
     </row>
-    <row r="90" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -5516,7 +5548,7 @@
       <c r="K90" s="2"/>
       <c r="L90" s="2"/>
     </row>
-    <row r="91" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -5530,7 +5562,7 @@
       <c r="K91" s="2"/>
       <c r="L91" s="2"/>
     </row>
-    <row r="92" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -5544,7 +5576,7 @@
       <c r="K92" s="2"/>
       <c r="L92" s="2"/>
     </row>
-    <row r="93" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -5558,7 +5590,7 @@
       <c r="K93" s="2"/>
       <c r="L93" s="2"/>
     </row>
-    <row r="94" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -5572,7 +5604,7 @@
       <c r="K94" s="2"/>
       <c r="L94" s="2"/>
     </row>
-    <row r="95" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -5586,7 +5618,7 @@
       <c r="K95" s="2"/>
       <c r="L95" s="2"/>
     </row>
-    <row r="96" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -5600,7 +5632,7 @@
       <c r="K96" s="2"/>
       <c r="L96" s="2"/>
     </row>
-    <row r="97" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -5614,7 +5646,7 @@
       <c r="K97" s="2"/>
       <c r="L97" s="2"/>
     </row>
-    <row r="98" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -5628,7 +5660,7 @@
       <c r="K98" s="2"/>
       <c r="L98" s="2"/>
     </row>
-    <row r="99" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -5642,7 +5674,7 @@
       <c r="K99" s="2"/>
       <c r="L99" s="2"/>
     </row>
-    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -5656,7 +5688,7 @@
       <c r="K100" s="2"/>
       <c r="L100" s="2"/>
     </row>
-    <row r="101" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -5670,7 +5702,7 @@
       <c r="K101" s="2"/>
       <c r="L101" s="2"/>
     </row>
-    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -5684,7 +5716,7 @@
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
     </row>
-    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -5698,7 +5730,7 @@
       <c r="K103" s="2"/>
       <c r="L103" s="2"/>
     </row>
-    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -5712,7 +5744,7 @@
       <c r="K104" s="2"/>
       <c r="L104" s="2"/>
     </row>
-    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -5726,7 +5758,7 @@
       <c r="K105" s="2"/>
       <c r="L105" s="2"/>
     </row>
-    <row r="106" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -5740,7 +5772,7 @@
       <c r="K106" s="2"/>
       <c r="L106" s="2"/>
     </row>
-    <row r="107" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -5754,7 +5786,7 @@
       <c r="K107" s="2"/>
       <c r="L107" s="2"/>
     </row>
-    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -5768,7 +5800,7 @@
       <c r="K108" s="2"/>
       <c r="L108" s="2"/>
     </row>
-    <row r="109" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -5782,7 +5814,7 @@
       <c r="K109" s="2"/>
       <c r="L109" s="2"/>
     </row>
-    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -5796,7 +5828,7 @@
       <c r="K110" s="2"/>
       <c r="L110" s="2"/>
     </row>
-    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -5810,7 +5842,7 @@
       <c r="K111" s="2"/>
       <c r="L111" s="2"/>
     </row>
-    <row r="112" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -5824,7 +5856,7 @@
       <c r="K112" s="2"/>
       <c r="L112" s="2"/>
     </row>
-    <row r="113" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -5838,7 +5870,7 @@
       <c r="K113" s="2"/>
       <c r="L113" s="2"/>
     </row>
-    <row r="114" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -5852,7 +5884,7 @@
       <c r="K114" s="2"/>
       <c r="L114" s="2"/>
     </row>
-    <row r="115" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -5866,7 +5898,7 @@
       <c r="K115" s="2"/>
       <c r="L115" s="2"/>
     </row>
-    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -5880,7 +5912,7 @@
       <c r="K116" s="2"/>
       <c r="L116" s="2"/>
     </row>
-    <row r="117" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -5894,7 +5926,7 @@
       <c r="K117" s="2"/>
       <c r="L117" s="2"/>
     </row>
-    <row r="118" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -5908,7 +5940,7 @@
       <c r="K118" s="2"/>
       <c r="L118" s="2"/>
     </row>
-    <row r="119" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -5922,7 +5954,7 @@
       <c r="K119" s="2"/>
       <c r="L119" s="2"/>
     </row>
-    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -5936,7 +5968,7 @@
       <c r="K120" s="2"/>
       <c r="L120" s="2"/>
     </row>
-    <row r="121" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -5950,7 +5982,7 @@
       <c r="K121" s="2"/>
       <c r="L121" s="2"/>
     </row>
-    <row r="122" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -5964,7 +5996,7 @@
       <c r="K122" s="2"/>
       <c r="L122" s="2"/>
     </row>
-    <row r="123" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -5978,7 +6010,7 @@
       <c r="K123" s="2"/>
       <c r="L123" s="2"/>
     </row>
-    <row r="124" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -5992,7 +6024,7 @@
       <c r="K124" s="2"/>
       <c r="L124" s="2"/>
     </row>
-    <row r="125" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -6006,7 +6038,7 @@
       <c r="K125" s="2"/>
       <c r="L125" s="2"/>
     </row>
-    <row r="126" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -6020,7 +6052,7 @@
       <c r="K126" s="2"/>
       <c r="L126" s="2"/>
     </row>
-    <row r="127" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -6034,7 +6066,7 @@
       <c r="K127" s="2"/>
       <c r="L127" s="2"/>
     </row>
-    <row r="128" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -6048,7 +6080,7 @@
       <c r="K128" s="2"/>
       <c r="L128" s="2"/>
     </row>
-    <row r="129" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -6062,7 +6094,7 @@
       <c r="K129" s="2"/>
       <c r="L129" s="2"/>
     </row>
-    <row r="130" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -6076,7 +6108,7 @@
       <c r="K130" s="2"/>
       <c r="L130" s="2"/>
     </row>
-    <row r="131" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -6090,7 +6122,7 @@
       <c r="K131" s="2"/>
       <c r="L131" s="2"/>
     </row>
-    <row r="132" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -6104,7 +6136,7 @@
       <c r="K132" s="2"/>
       <c r="L132" s="2"/>
     </row>
-    <row r="133" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>

</xml_diff>